<commit_message>
Found zscores for particular statistics
</commit_message>
<xml_diff>
--- a/3rd_Q_Statistics.xlsx
+++ b/3rd_Q_Statistics.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shubhan/Desktop/Projects/3rd_q_statistics/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8137227A-0E5F-CB4E-BD0A-0BEFBFF5C779}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F20BCA35-2289-084B-8264-2C99DFF9BC3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="28800" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,6 +28,7 @@
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
         <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="173">
   <si>
     <t>Name</t>
   </si>
@@ -118,427 +119,442 @@
     <t>3s Missed</t>
   </si>
   <si>
+    <t>Total Shots</t>
+  </si>
+  <si>
+    <t>Total 3s</t>
+  </si>
+  <si>
+    <t>Shooting % Total Game</t>
+  </si>
+  <si>
+    <t>Assist/Turnover Ratio Game</t>
+  </si>
+  <si>
+    <t>3 % Entire Game</t>
+  </si>
+  <si>
+    <t>Z-Score for PPQ</t>
+  </si>
+  <si>
+    <t>Z-Score for APQ</t>
+  </si>
+  <si>
+    <t>Z-Score for ATRPQ</t>
+  </si>
+  <si>
+    <t>Z-Score for SPQ</t>
+  </si>
+  <si>
+    <t>Z-Score for BPQ</t>
+  </si>
+  <si>
+    <t>M. Turner</t>
+  </si>
+  <si>
+    <t>A. Davis</t>
+  </si>
+  <si>
+    <t>M. Robinson</t>
+  </si>
+  <si>
+    <t>E. Mobley</t>
+  </si>
+  <si>
+    <t>R. Williams</t>
+  </si>
+  <si>
+    <t>J. Jackson</t>
+  </si>
+  <si>
+    <t>J. Embiid</t>
+  </si>
+  <si>
+    <t>B. Lopez</t>
+  </si>
+  <si>
+    <t>G. Antetokounmpo</t>
+  </si>
+  <si>
+    <t>R. Gobert</t>
+  </si>
+  <si>
+    <t>A. Horford</t>
+  </si>
+  <si>
+    <t>C. Capela</t>
+  </si>
+  <si>
+    <t>J. Poeltl</t>
+  </si>
+  <si>
+    <t>J. Allen</t>
+  </si>
+  <si>
+    <t>J. Grant</t>
+  </si>
+  <si>
+    <t>L. James</t>
+  </si>
+  <si>
+    <t>J. Collins</t>
+  </si>
+  <si>
+    <t>M. Bamba</t>
+  </si>
+  <si>
+    <t>A. Drummond</t>
+  </si>
+  <si>
+    <t>I. Zubac</t>
+  </si>
+  <si>
+    <t>K. Towns</t>
+  </si>
+  <si>
+    <t>S. Adams</t>
+  </si>
+  <si>
+    <t>A. Wiggins</t>
+  </si>
+  <si>
+    <t>M. Bridges</t>
+  </si>
+  <si>
+    <t>K. Durant</t>
+  </si>
+  <si>
+    <t>C. Cunningham</t>
+  </si>
+  <si>
+    <t>I. Stewart</t>
+  </si>
+  <si>
+    <t>K. Porziņģis</t>
+  </si>
+  <si>
+    <t>N. Batum</t>
+  </si>
+  <si>
+    <t>S. Gilgeous-Alexander</t>
+  </si>
+  <si>
+    <t>N. Jokić</t>
+  </si>
+  <si>
+    <t>D. Ayton</t>
+  </si>
+  <si>
+    <t>D. Green</t>
+  </si>
+  <si>
+    <t>J. Tatum</t>
+  </si>
+  <si>
+    <t>J. Valančiūnas</t>
+  </si>
+  <si>
+    <t>N. Vučević</t>
+  </si>
+  <si>
+    <t>K. Looney</t>
+  </si>
+  <si>
+    <t>H. Jones</t>
+  </si>
+  <si>
+    <t>B. Brown</t>
+  </si>
+  <si>
+    <t>J. Vanderbilt</t>
+  </si>
+  <si>
+    <t>L. Dončić</t>
+  </si>
+  <si>
+    <t>B. Ingram</t>
+  </si>
+  <si>
+    <t>T. Harris</t>
+  </si>
+  <si>
+    <t>K. Kuzma</t>
+  </si>
+  <si>
+    <t>D. Sabonis</t>
+  </si>
+  <si>
+    <t>P. Washington</t>
+  </si>
+  <si>
+    <t>A. Gordon</t>
+  </si>
+  <si>
+    <t>B. Portis</t>
+  </si>
+  <si>
+    <t>P. Siakam</t>
+  </si>
+  <si>
+    <t>S. Barnes</t>
+  </si>
+  <si>
+    <t>D. Finney-Smith</t>
+  </si>
+  <si>
+    <t>M. Brogdon</t>
+  </si>
+  <si>
+    <t>J. Holiday</t>
+  </si>
+  <si>
+    <t>K. Irving</t>
+  </si>
+  <si>
+    <t>J. Randle</t>
+  </si>
+  <si>
+    <t>J. Nurkić</t>
+  </si>
+  <si>
+    <t>D. Powell</t>
+  </si>
+  <si>
+    <t>A. Edwards</t>
+  </si>
+  <si>
+    <t>T. Haliburton</t>
+  </si>
+  <si>
+    <t>B. Hield</t>
+  </si>
+  <si>
+    <t>W. Carter</t>
+  </si>
+  <si>
+    <t>D. Bazley</t>
+  </si>
+  <si>
+    <t>L. Dort</t>
+  </si>
+  <si>
+    <t>T. Rozier</t>
+  </si>
+  <si>
+    <t>D. Booker</t>
+  </si>
+  <si>
+    <t>P. Williams</t>
+  </si>
+  <si>
+    <t>J. Butler</t>
+  </si>
+  <si>
+    <t>J. Suggs</t>
+  </si>
+  <si>
+    <t>S. Curry</t>
+  </si>
+  <si>
+    <t>B. Adebayo</t>
+  </si>
+  <si>
+    <t>G. Hayward</t>
+  </si>
+  <si>
+    <t>F. VanVleet</t>
+  </si>
+  <si>
+    <t>C. Anthony</t>
+  </si>
+  <si>
+    <t>Z. LaVine</t>
+  </si>
+  <si>
+    <t>T. Maxey</t>
+  </si>
+  <si>
+    <t>D. Bane</t>
+  </si>
+  <si>
+    <t>D. DeRozan</t>
+  </si>
+  <si>
+    <t>D. Murray</t>
+  </si>
+  <si>
+    <t>L. Markkanen</t>
+  </si>
+  <si>
+    <t>W. Barton</t>
+  </si>
+  <si>
+    <t>E. Fournier</t>
+  </si>
+  <si>
+    <t>K. Hayes</t>
+  </si>
+  <si>
+    <t>B. Bogdanović</t>
+  </si>
+  <si>
+    <t>J. Morant</t>
+  </si>
+  <si>
+    <t>K. Porter</t>
+  </si>
+  <si>
+    <t>D. Mitchell</t>
+  </si>
+  <si>
+    <t>K. Oubre</t>
+  </si>
+  <si>
+    <t>J. Poole</t>
+  </si>
+  <si>
+    <t>A. Caruso</t>
+  </si>
+  <si>
+    <t>M. Smart</t>
+  </si>
+  <si>
+    <t>B. Beal</t>
+  </si>
+  <si>
+    <t>D. Vassell</t>
+  </si>
+  <si>
+    <t>M. Conley</t>
+  </si>
+  <si>
+    <t>K. Lowry</t>
+  </si>
+  <si>
+    <t>C. LeVert</t>
+  </si>
+  <si>
+    <t>P. George</t>
+  </si>
+  <si>
+    <t>R. Holmes</t>
+  </si>
+  <si>
+    <t>D. Hunter</t>
+  </si>
+  <si>
+    <t>R. Bullock</t>
+  </si>
+  <si>
+    <t>J. Harden</t>
+  </si>
+  <si>
+    <t>O. Anunoby</t>
+  </si>
+  <si>
+    <t>F. Wagner</t>
+  </si>
+  <si>
+    <t>C. Paul</t>
+  </si>
+  <si>
+    <t>J. Giddey</t>
+  </si>
+  <si>
+    <t>C. Duarte</t>
+  </si>
+  <si>
+    <t>J. Green</t>
+  </si>
+  <si>
+    <t>R. Hachimura</t>
+  </si>
+  <si>
+    <t>J. Hart</t>
+  </si>
+  <si>
+    <t>M. Morris</t>
+  </si>
+  <si>
+    <t>E. Gordon</t>
+  </si>
+  <si>
+    <t>D. Fox</t>
+  </si>
+  <si>
+    <t>L. Ball</t>
+  </si>
+  <si>
+    <t>K. Johnson</t>
+  </si>
+  <si>
+    <t>H. Barnes</t>
+  </si>
+  <si>
+    <t>K. Love</t>
+  </si>
+  <si>
+    <t>J. Tate</t>
+  </si>
+  <si>
     <t>T. Young</t>
   </si>
   <si>
+    <t>R. Westbrook</t>
+  </si>
+  <si>
+    <t>D. Brooks</t>
+  </si>
+  <si>
+    <t>S. Bey</t>
+  </si>
+  <si>
+    <t>K. Middleton</t>
+  </si>
+  <si>
+    <t>R. Barrett</t>
+  </si>
+  <si>
+    <t>G. Trent</t>
+  </si>
+  <si>
     <t>K. Huerter</t>
   </si>
   <si>
-    <t>D. Hunter</t>
+    <t>D. Russell</t>
+  </si>
+  <si>
+    <t>J. Brown</t>
+  </si>
+  <si>
+    <t>D. Lillard</t>
+  </si>
+  <si>
+    <t>K. Thompson</t>
   </si>
   <si>
     <t>D. Gallinari</t>
   </si>
   <si>
-    <t>J. Collins</t>
-  </si>
-  <si>
-    <t>B. Bogdanović</t>
-  </si>
-  <si>
-    <t>C. Capela</t>
-  </si>
-  <si>
-    <t>M. Smart</t>
-  </si>
-  <si>
-    <t>J. Brown</t>
-  </si>
-  <si>
-    <t>J. Tatum</t>
-  </si>
-  <si>
-    <t>A. Horford</t>
-  </si>
-  <si>
-    <t>R. Williams</t>
-  </si>
-  <si>
-    <t>K. Irving</t>
-  </si>
-  <si>
-    <t>S. Curry</t>
-  </si>
-  <si>
-    <t>B. Brown</t>
-  </si>
-  <si>
-    <t>K. Durant</t>
-  </si>
-  <si>
-    <t>A. Drummond</t>
-  </si>
-  <si>
-    <t>L. Ball</t>
-  </si>
-  <si>
-    <t>T. Rozier</t>
-  </si>
-  <si>
-    <t>G. Hayward</t>
-  </si>
-  <si>
-    <t>M. Bridges</t>
-  </si>
-  <si>
-    <t>K. Oubre</t>
-  </si>
-  <si>
-    <t>P. Washington</t>
-  </si>
-  <si>
-    <t>A. Caruso</t>
-  </si>
-  <si>
-    <t>Z. LaVine</t>
-  </si>
-  <si>
-    <t>D. DeRozan</t>
-  </si>
-  <si>
-    <t>P. Williams</t>
-  </si>
-  <si>
-    <t>N. Vučević</t>
+    <t>R. Jackson</t>
+  </si>
+  <si>
+    <t>J. Clarkson</t>
+  </si>
+  <si>
+    <t>T. Herro</t>
   </si>
   <si>
     <t>D. Garland</t>
   </si>
   <si>
-    <t>C. LeVert</t>
-  </si>
-  <si>
-    <t>L. Markkanen</t>
-  </si>
-  <si>
-    <t>E. Mobley</t>
-  </si>
-  <si>
-    <t>J. Allen</t>
-  </si>
-  <si>
-    <t>K. Love</t>
-  </si>
-  <si>
-    <t>L. Dončić</t>
+    <t>C. McCollum</t>
   </si>
   <si>
     <t>J. Brunson</t>
   </si>
   <si>
-    <t>R. Bullock</t>
-  </si>
-  <si>
-    <t>D. Finney-Smith</t>
-  </si>
-  <si>
-    <t>D. Powell</t>
-  </si>
-  <si>
-    <t>M. Morris</t>
-  </si>
-  <si>
-    <t>W. Barton</t>
-  </si>
-  <si>
-    <t>A. Gordon</t>
-  </si>
-  <si>
-    <t>N. Jokić</t>
-  </si>
-  <si>
-    <t>K. Hayes</t>
-  </si>
-  <si>
-    <t>C. Cunningham</t>
-  </si>
-  <si>
-    <t>S. Bey</t>
-  </si>
-  <si>
-    <t>J. Grant</t>
-  </si>
-  <si>
-    <t>I. Stewart</t>
-  </si>
-  <si>
-    <t>K. Thompson</t>
-  </si>
-  <si>
-    <t>A. Wiggins</t>
-  </si>
-  <si>
-    <t>D. Green</t>
-  </si>
-  <si>
-    <t>K. Looney</t>
-  </si>
-  <si>
-    <t>J. Poole</t>
-  </si>
-  <si>
-    <t>K. Porter</t>
-  </si>
-  <si>
-    <t>J. Green</t>
-  </si>
-  <si>
-    <t>E. Gordon</t>
-  </si>
-  <si>
-    <t>J. Tate</t>
-  </si>
-  <si>
-    <t>M. Brogdon</t>
-  </si>
-  <si>
-    <t>B. Hield</t>
-  </si>
-  <si>
-    <t>T. Haliburton</t>
-  </si>
-  <si>
-    <t>C. Duarte</t>
-  </si>
-  <si>
-    <t>M. Turner</t>
-  </si>
-  <si>
-    <t>R. Jackson</t>
-  </si>
-  <si>
-    <t>N. Batum</t>
-  </si>
-  <si>
-    <t>P. George</t>
-  </si>
-  <si>
-    <t>I. Zubac</t>
-  </si>
-  <si>
-    <t>R. Westbrook</t>
-  </si>
-  <si>
-    <t>L. James</t>
-  </si>
-  <si>
-    <t>A. Davis</t>
-  </si>
-  <si>
-    <t>J. Morant</t>
-  </si>
-  <si>
-    <t>D. Brooks</t>
-  </si>
-  <si>
-    <t>D. Bane</t>
-  </si>
-  <si>
-    <t>J. Jackson</t>
-  </si>
-  <si>
-    <t>S. Adams</t>
-  </si>
-  <si>
-    <t>K. Lowry</t>
-  </si>
-  <si>
-    <t>T. Herro</t>
-  </si>
-  <si>
-    <t>J. Butler</t>
-  </si>
-  <si>
-    <t>B. Adebayo</t>
-  </si>
-  <si>
-    <t>J. Holiday</t>
-  </si>
-  <si>
-    <t>K. Middleton</t>
-  </si>
-  <si>
-    <t>G. Antetokounmpo</t>
-  </si>
-  <si>
-    <t>B. Portis</t>
-  </si>
-  <si>
-    <t>B. Lopez</t>
-  </si>
-  <si>
-    <t>D. Russell</t>
-  </si>
-  <si>
-    <t>A. Edwards</t>
-  </si>
-  <si>
-    <t>K. Towns</t>
-  </si>
-  <si>
-    <t>J. Vanderbilt</t>
-  </si>
-  <si>
-    <t>C. McCollum</t>
-  </si>
-  <si>
-    <t>H. Jones</t>
-  </si>
-  <si>
-    <t>B. Ingram</t>
-  </si>
-  <si>
-    <t>J. Valančiūnas</t>
-  </si>
-  <si>
-    <t>R. Barrett</t>
-  </si>
-  <si>
-    <t>J. Randle</t>
-  </si>
-  <si>
-    <t>M. Robinson</t>
-  </si>
-  <si>
-    <t>E. Fournier</t>
-  </si>
-  <si>
-    <t>S. Gilgeous-Alexander</t>
-  </si>
-  <si>
-    <t>L. Dort</t>
-  </si>
-  <si>
-    <t>J. Giddey</t>
-  </si>
-  <si>
-    <t>D. Bazley</t>
-  </si>
-  <si>
-    <t>C. Anthony</t>
-  </si>
-  <si>
-    <t>J. Suggs</t>
-  </si>
-  <si>
-    <t>F. Wagner</t>
-  </si>
-  <si>
-    <t>W. Carter</t>
-  </si>
-  <si>
-    <t>M. Bamba</t>
-  </si>
-  <si>
-    <t>J. Harden</t>
-  </si>
-  <si>
-    <t>T. Maxey</t>
-  </si>
-  <si>
-    <t>T. Harris</t>
-  </si>
-  <si>
-    <t>J. Embiid</t>
-  </si>
-  <si>
-    <t>C. Paul</t>
-  </si>
-  <si>
-    <t>D. Booker</t>
-  </si>
-  <si>
-    <t>D. Ayton</t>
-  </si>
-  <si>
-    <t>D. Lillard</t>
-  </si>
-  <si>
     <t>A. Simons</t>
-  </si>
-  <si>
-    <t>J. Hart</t>
-  </si>
-  <si>
-    <t>J. Nurkić</t>
-  </si>
-  <si>
-    <t>D. Fox</t>
-  </si>
-  <si>
-    <t>D. Mitchell</t>
-  </si>
-  <si>
-    <t>H. Barnes</t>
-  </si>
-  <si>
-    <t>D. Sabonis</t>
-  </si>
-  <si>
-    <t>R. Holmes</t>
-  </si>
-  <si>
-    <t>D. Murray</t>
-  </si>
-  <si>
-    <t>K. Johnson</t>
-  </si>
-  <si>
-    <t>D. Vassell</t>
-  </si>
-  <si>
-    <t>J. Poeltl</t>
-  </si>
-  <si>
-    <t>F. VanVleet</t>
-  </si>
-  <si>
-    <t>G. Trent</t>
-  </si>
-  <si>
-    <t>O. Anunoby</t>
-  </si>
-  <si>
-    <t>P. Siakam</t>
-  </si>
-  <si>
-    <t>S. Barnes</t>
-  </si>
-  <si>
-    <t>M. Conley</t>
-  </si>
-  <si>
-    <t>J. Clarkson</t>
-  </si>
-  <si>
-    <t>R. Gobert</t>
-  </si>
-  <si>
-    <t>B. Beal</t>
-  </si>
-  <si>
-    <t>K. Kuzma</t>
-  </si>
-  <si>
-    <t>K. Porziņģis</t>
-  </si>
-  <si>
-    <t>R. Hachimura</t>
-  </si>
-  <si>
-    <t>Total Shots</t>
-  </si>
-  <si>
-    <t>Total 3s</t>
-  </si>
-  <si>
-    <t>Shooting % Total Game</t>
-  </si>
-  <si>
-    <t>Assist/Turnover Ratio Game</t>
-  </si>
-  <si>
-    <t>3 % Entire Game</t>
   </si>
 </sst>
 </file>
@@ -912,10 +928,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AF142"/>
+  <dimension ref="A1:AK142"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AB1" workbookViewId="0">
-      <selection activeCell="AJ23" sqref="AJ23"/>
+    <sheetView tabSelected="1" topLeftCell="AC1" workbookViewId="0">
+      <selection activeCell="AH6" sqref="AH6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -937,9 +953,14 @@
     <col min="30" max="30" width="21.5" customWidth="1"/>
     <col min="31" max="31" width="21.33203125" customWidth="1"/>
     <col min="32" max="32" width="22" customWidth="1"/>
+    <col min="33" max="33" width="28.33203125" customWidth="1"/>
+    <col min="34" max="34" width="27" customWidth="1"/>
+    <col min="35" max="35" width="21" customWidth="1"/>
+    <col min="36" max="36" width="19.83203125" customWidth="1"/>
+    <col min="37" max="37" width="22" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1022,24 +1043,39 @@
         <v>26</v>
       </c>
       <c r="AB1" s="1" t="s">
-        <v>163</v>
+        <v>27</v>
       </c>
       <c r="AC1" s="1" t="s">
-        <v>164</v>
+        <v>28</v>
       </c>
       <c r="AD1" s="1" t="s">
-        <v>165</v>
+        <v>29</v>
       </c>
       <c r="AE1" s="1" t="s">
-        <v>166</v>
+        <v>30</v>
       </c>
       <c r="AF1" s="1" t="s">
-        <v>167</v>
+        <v>31</v>
+      </c>
+      <c r="AG1" t="s">
+        <v>32</v>
+      </c>
+      <c r="AH1" t="s">
+        <v>33</v>
+      </c>
+      <c r="AI1" t="s">
+        <v>34</v>
+      </c>
+      <c r="AJ1" t="s">
+        <v>35</v>
+      </c>
+      <c r="AK1" t="s">
+        <v>36</v>
       </c>
     </row>
-    <row r="2" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>88</v>
+        <v>37</v>
       </c>
       <c r="B2">
         <v>150</v>
@@ -1127,10 +1163,25 @@
         <f t="shared" ref="AC2:AC33" si="1">SUM(Z2,AA2)</f>
         <v>80</v>
       </c>
+      <c r="AG2">
+        <v>-0.6405783235404765</v>
+      </c>
+      <c r="AH2">
+        <v>-1.3215935728857471</v>
+      </c>
+      <c r="AI2">
+        <v>-1.7489466668762319</v>
+      </c>
+      <c r="AJ2">
+        <v>-0.12707806957341289</v>
+      </c>
+      <c r="AK2">
+        <v>5.0794407987865906</v>
+      </c>
     </row>
-    <row r="3" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>95</v>
+        <v>38</v>
       </c>
       <c r="B3">
         <v>261</v>
@@ -1221,10 +1272,25 @@
       <c r="AD3">
         <v>53.2</v>
       </c>
+      <c r="AG3">
+        <v>1.284502708352919</v>
+      </c>
+      <c r="AH3">
+        <v>0.1011261916901965</v>
+      </c>
+      <c r="AI3">
+        <v>-0.1914956472252618</v>
+      </c>
+      <c r="AJ3">
+        <v>0.79383576056748784</v>
+      </c>
+      <c r="AK3">
+        <v>4.0945691181057358</v>
+      </c>
     </row>
-    <row r="4" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>120</v>
+        <v>39</v>
       </c>
       <c r="B4">
         <v>149</v>
@@ -1312,10 +1378,25 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
+      <c r="AG4">
+        <v>-1.5005531735115161</v>
+      </c>
+      <c r="AH4">
+        <v>-1.479189926396554</v>
+      </c>
+      <c r="AI4">
+        <v>-1.657761009988002</v>
+      </c>
+      <c r="AJ4">
+        <v>-0.5648745531979773</v>
+      </c>
+      <c r="AK4">
+        <v>2.509174906963612</v>
+      </c>
     </row>
-    <row r="5" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>58</v>
+        <v>40</v>
       </c>
       <c r="B5">
         <v>280</v>
@@ -1403,10 +1484,25 @@
         <f t="shared" si="1"/>
         <v>28</v>
       </c>
+      <c r="AG5">
+        <v>-0.39033974014726458</v>
+      </c>
+      <c r="AH5">
+        <v>-0.76766579569429338</v>
+      </c>
+      <c r="AI5">
+        <v>-1.1997121288750321</v>
+      </c>
+      <c r="AJ5">
+        <v>-0.78580231513302246</v>
+      </c>
+      <c r="AK5">
+        <v>2.462994086039751</v>
+      </c>
     </row>
-    <row r="6" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="B6">
         <v>147</v>
@@ -1494,10 +1590,25 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
+      <c r="AG6">
+        <v>-1.295369283419382</v>
+      </c>
+      <c r="AH6">
+        <v>-0.72335157351897716</v>
+      </c>
+      <c r="AI6">
+        <v>-0.47234747044101072</v>
+      </c>
+      <c r="AJ6">
+        <v>0.49047591063872042</v>
+      </c>
+      <c r="AK6">
+        <v>2.2642766141855608</v>
+      </c>
     </row>
-    <row r="7" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>99</v>
+        <v>42</v>
       </c>
       <c r="B7">
         <v>322</v>
@@ -1585,10 +1696,25 @@
         <f t="shared" si="1"/>
         <v>118</v>
       </c>
+      <c r="AG7">
+        <v>-0.31548204426040599</v>
+      </c>
+      <c r="AH7">
+        <v>-1.29602767547691</v>
+      </c>
+      <c r="AI7">
+        <v>-1.388168633101061</v>
+      </c>
+      <c r="AJ7">
+        <v>-0.17458222189742351</v>
+      </c>
+      <c r="AK7">
+        <v>2.1751085178407319</v>
+      </c>
     </row>
-    <row r="8" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>134</v>
+        <v>43</v>
       </c>
       <c r="B8">
         <v>638</v>
@@ -1679,10 +1805,25 @@
       <c r="AD8" s="2">
         <v>49.9</v>
       </c>
+      <c r="AG8">
+        <v>2.752362468938077</v>
+      </c>
+      <c r="AH8">
+        <v>0.21637060849287579</v>
+      </c>
+      <c r="AI8">
+        <v>-0.87012837947517407</v>
+      </c>
+      <c r="AJ8">
+        <v>-0.1028602664278392</v>
+      </c>
+      <c r="AK8">
+        <v>2.1619955624959042</v>
+      </c>
     </row>
-    <row r="9" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>109</v>
+        <v>44</v>
       </c>
       <c r="B9">
         <v>59</v>
@@ -1770,10 +1911,25 @@
         <f t="shared" si="1"/>
         <v>17</v>
       </c>
+      <c r="AG9">
+        <v>-7.5937417422459588E-2</v>
+      </c>
+      <c r="AH9">
+        <v>-1.176720154235674</v>
+      </c>
+      <c r="AI9">
+        <v>0.16595212777659979</v>
+      </c>
+      <c r="AJ9">
+        <v>0.26878986646000608</v>
+      </c>
+      <c r="AK9">
+        <v>1.9967723251510741</v>
+      </c>
     </row>
-    <row r="10" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>107</v>
+        <v>45</v>
       </c>
       <c r="B10">
         <v>551</v>
@@ -1864,10 +2020,25 @@
       <c r="AD10" s="2">
         <v>55.3</v>
       </c>
+      <c r="AG10">
+        <v>2.0759420195639469</v>
+      </c>
+      <c r="AH10">
+        <v>0.56837493257643534</v>
+      </c>
+      <c r="AI10">
+        <v>-0.1987904997763203</v>
+      </c>
+      <c r="AJ10">
+        <v>0.1893799401870328</v>
+      </c>
+      <c r="AK10">
+        <v>1.9009498932581239</v>
+      </c>
     </row>
-    <row r="11" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>158</v>
+        <v>46</v>
       </c>
       <c r="B11">
         <v>236</v>
@@ -1955,10 +2126,25 @@
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
+      <c r="AG11">
+        <v>-0.63805066108195929</v>
+      </c>
+      <c r="AH11">
+        <v>-1.324950710929331</v>
+      </c>
+      <c r="AI11">
+        <v>-1.725305941016321</v>
+      </c>
+      <c r="AJ11">
+        <v>-3.3509284692786918E-2</v>
+      </c>
+      <c r="AK11">
+        <v>1.842754704191824</v>
+      </c>
     </row>
-    <row r="12" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>37</v>
+        <v>47</v>
       </c>
       <c r="B12">
         <v>251</v>
@@ -2046,10 +2232,25 @@
         <f t="shared" si="1"/>
         <v>140</v>
       </c>
+      <c r="AG12">
+        <v>-0.60189409808838601</v>
+      </c>
+      <c r="AH12">
+        <v>-3.5517777145590269E-2</v>
+      </c>
+      <c r="AI12">
+        <v>1.989665265541203</v>
+      </c>
+      <c r="AJ12">
+        <v>-0.51193054999546717</v>
+      </c>
+      <c r="AK12">
+        <v>1.508286232131576</v>
+      </c>
     </row>
-    <row r="13" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>33</v>
+        <v>48</v>
       </c>
       <c r="B13">
         <v>241</v>
@@ -2137,10 +2338,25 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
+      <c r="AG13">
+        <v>-0.8496665621090278</v>
+      </c>
+      <c r="AH13">
+        <v>-0.86811136595834348</v>
+      </c>
+      <c r="AI13">
+        <v>0.84680503254205231</v>
+      </c>
+      <c r="AJ13">
+        <v>-8.5907804225937037E-2</v>
+      </c>
+      <c r="AK13">
+        <v>1.38329582229865</v>
+      </c>
     </row>
-    <row r="14" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>150</v>
+        <v>49</v>
       </c>
       <c r="B14">
         <v>218</v>
@@ -2228,10 +2444,25 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
+      <c r="AG14">
+        <v>-0.85401711525821633</v>
+      </c>
+      <c r="AH14">
+        <v>-0.51351069792409709</v>
+      </c>
+      <c r="AI14">
+        <v>-0.32821530310154989</v>
+      </c>
+      <c r="AJ14">
+        <v>-0.86572106551341621</v>
+      </c>
+      <c r="AK14">
+        <v>1.343747148978649</v>
+      </c>
     </row>
-    <row r="15" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>59</v>
+        <v>50</v>
       </c>
       <c r="B15">
         <v>200</v>
@@ -2319,10 +2550,25 @@
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
+      <c r="AG15">
+        <v>-0.6405783235404765</v>
+      </c>
+      <c r="AH15">
+        <v>-0.87845135113258399</v>
+      </c>
+      <c r="AI15">
+        <v>-1.154667730604664</v>
+      </c>
+      <c r="AJ15">
+        <v>-1.1563347032603031</v>
+      </c>
+      <c r="AK15">
+        <v>1.2706892549146089</v>
+      </c>
     </row>
-    <row r="16" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>73</v>
+        <v>51</v>
       </c>
       <c r="B16">
         <v>266</v>
@@ -2410,10 +2656,25 @@
         <f t="shared" si="1"/>
         <v>117</v>
       </c>
+      <c r="AG16">
+        <v>0.65050770092305288</v>
+      </c>
+      <c r="AH16">
+        <v>-0.54127792153778642</v>
+      </c>
+      <c r="AI16">
+        <v>-0.98298714901509943</v>
+      </c>
+      <c r="AJ16">
+        <v>-0.32397933862655698</v>
+      </c>
+      <c r="AK16">
+        <v>1.2058900793099809</v>
+      </c>
     </row>
-    <row r="17" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>94</v>
+        <v>52</v>
       </c>
       <c r="B17">
         <v>393</v>
@@ -2501,10 +2762,25 @@
         <f t="shared" si="1"/>
         <v>173</v>
       </c>
+      <c r="AG17">
+        <v>1.371756951246605</v>
+      </c>
+      <c r="AH17">
+        <v>0.45097531412690361</v>
+      </c>
+      <c r="AI17">
+        <v>-0.36596420407140862</v>
+      </c>
+      <c r="AJ17">
+        <v>0.54193874232306527</v>
+      </c>
+      <c r="AK17">
+        <v>1.1464908350057399</v>
+      </c>
     </row>
-    <row r="18" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>31</v>
+        <v>53</v>
       </c>
       <c r="B18">
         <v>263</v>
@@ -2595,10 +2871,25 @@
       <c r="AD18">
         <v>52.6</v>
       </c>
+      <c r="AG18">
+        <v>0.1178608397068515</v>
+      </c>
+      <c r="AH18">
+        <v>-0.76356262697435673</v>
+      </c>
+      <c r="AI18">
+        <v>-5.9330083359026807E-2</v>
+      </c>
+      <c r="AJ18">
+        <v>-1.5909097263725449</v>
+      </c>
+      <c r="AK18">
+        <v>1.1050913617027831</v>
+      </c>
     </row>
-    <row r="19" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>130</v>
+        <v>54</v>
       </c>
       <c r="B19">
         <v>186</v>
@@ -2686,10 +2977,25 @@
         <f t="shared" si="1"/>
         <v>102</v>
       </c>
+      <c r="AG19">
+        <v>-1.17442063477933</v>
+      </c>
+      <c r="AH19">
+        <v>-1.100022462009165</v>
+      </c>
+      <c r="AI19">
+        <v>-0.70751048031065611</v>
+      </c>
+      <c r="AJ19">
+        <v>-1.526867091387583</v>
+      </c>
+      <c r="AK19">
+        <v>1.071971783060419</v>
+      </c>
     </row>
-    <row r="20" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>43</v>
+        <v>55</v>
       </c>
       <c r="B20">
         <v>80</v>
@@ -2777,10 +3083,25 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
+      <c r="AG20">
+        <v>-1.057642629195831</v>
+      </c>
+      <c r="AH20">
+        <v>-0.71227301797514808</v>
+      </c>
+      <c r="AI20">
+        <v>-0.7178473159093226</v>
+      </c>
+      <c r="AJ20">
+        <v>-0.53878072304816871</v>
+      </c>
+      <c r="AK20">
+        <v>1.0222924150968711</v>
+      </c>
     </row>
-    <row r="21" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>92</v>
+        <v>56</v>
       </c>
       <c r="B21">
         <v>247</v>
@@ -2868,10 +3189,25 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
+      <c r="AG21">
+        <v>-0.828257261085386</v>
+      </c>
+      <c r="AH21">
+        <v>-0.89885921660805856</v>
+      </c>
+      <c r="AI21">
+        <v>-1.3137423953642251</v>
+      </c>
+      <c r="AJ21">
+        <v>-0.57128356411196524</v>
+      </c>
+      <c r="AK21">
+        <v>0.98307186144143832</v>
+      </c>
     </row>
-    <row r="22" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>112</v>
+        <v>57</v>
       </c>
       <c r="B22">
         <v>553</v>
@@ -2962,10 +3298,25 @@
       <c r="AD22" s="2">
         <v>52.9</v>
       </c>
+      <c r="AG22">
+        <v>1.5793159540277519</v>
+      </c>
+      <c r="AH22">
+        <v>0.2279270625111447</v>
+      </c>
+      <c r="AI22">
+        <v>-0.31277257088660848</v>
+      </c>
+      <c r="AJ22">
+        <v>-8.5907804225937037E-2</v>
+      </c>
+      <c r="AK22">
+        <v>0.91962172130553843</v>
+      </c>
     </row>
-    <row r="23" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>100</v>
+        <v>58</v>
       </c>
       <c r="B23">
         <v>140</v>
@@ -3053,10 +3404,25 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
+      <c r="AG23">
+        <v>-1.650312958285018</v>
+      </c>
+      <c r="AH23">
+        <v>-0.1233603285400241</v>
+      </c>
+      <c r="AI23">
+        <v>0.20045480876133609</v>
+      </c>
+      <c r="AJ23">
+        <v>-0.57128356411196524</v>
+      </c>
+      <c r="AK23">
+        <v>0.8915572362454296</v>
+      </c>
     </row>
-    <row r="24" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>76</v>
+        <v>59</v>
       </c>
       <c r="B24">
         <v>363</v>
@@ -3144,10 +3510,25 @@
         <f t="shared" si="1"/>
         <v>152</v>
       </c>
+      <c r="AG24">
+        <v>0.1775533007039978</v>
+      </c>
+      <c r="AH24">
+        <v>-0.80408844405756708</v>
+      </c>
+      <c r="AI24">
+        <v>-0.62641978725215774</v>
+      </c>
+      <c r="AJ24">
+        <v>0.33256256410045798</v>
+      </c>
+      <c r="AK24">
+        <v>0.88278186122663416</v>
+      </c>
     </row>
-    <row r="25" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>47</v>
+        <v>60</v>
       </c>
       <c r="B25">
         <v>445</v>
@@ -3235,10 +3616,25 @@
         <f t="shared" si="1"/>
         <v>168</v>
       </c>
+      <c r="AG25">
+        <v>0.48189104229738899</v>
+      </c>
+      <c r="AH25">
+        <v>8.8528743865829665E-2</v>
+      </c>
+      <c r="AI25">
+        <v>0.66987286321155748</v>
+      </c>
+      <c r="AJ25">
+        <v>-0.25668816418583612</v>
+      </c>
+      <c r="AK25">
+        <v>0.8474946389288327</v>
+      </c>
     </row>
-    <row r="26" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>42</v>
+        <v>61</v>
       </c>
       <c r="B26">
         <v>495</v>
@@ -3332,10 +3728,25 @@
       <c r="AE26">
         <v>1.83</v>
       </c>
+      <c r="AG26">
+        <v>2.5291103994402109</v>
+      </c>
+      <c r="AH26">
+        <v>1.532645191769852</v>
+      </c>
+      <c r="AI26">
+        <v>0.1435556506461598</v>
+      </c>
+      <c r="AJ26">
+        <v>-0.19070484329223919</v>
+      </c>
+      <c r="AK26">
+        <v>0.81002602470716722</v>
+      </c>
     </row>
-    <row r="27" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
       <c r="B27">
         <v>303</v>
@@ -3423,10 +3834,25 @@
         <f t="shared" si="1"/>
         <v>131</v>
       </c>
+      <c r="AG27">
+        <v>8.2333139595469479E-2</v>
+      </c>
+      <c r="AH27">
+        <v>0.63561790652405481</v>
+      </c>
+      <c r="AI27">
+        <v>-0.71508112046742611</v>
+      </c>
+      <c r="AJ27">
+        <v>0.76494434628855812</v>
+      </c>
+      <c r="AK27">
+        <v>0.77389557527913255</v>
+      </c>
     </row>
-    <row r="28" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>74</v>
+        <v>63</v>
       </c>
       <c r="B28">
         <v>142</v>
@@ -3514,10 +3940,25 @@
         <f t="shared" si="1"/>
         <v>14</v>
       </c>
+      <c r="AG28">
+        <v>-1.5066000876365939</v>
+      </c>
+      <c r="AH28">
+        <v>-1.106539259387888</v>
+      </c>
+      <c r="AI28">
+        <v>-0.92827575488216096</v>
+      </c>
+      <c r="AJ28">
+        <v>-1.7557253311132559</v>
+      </c>
+      <c r="AK28">
+        <v>0.73006083884070871</v>
+      </c>
     </row>
-    <row r="29" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>161</v>
+        <v>64</v>
       </c>
       <c r="B29">
         <v>106</v>
@@ -3605,10 +4046,25 @@
         <f t="shared" si="1"/>
         <v>33</v>
       </c>
+      <c r="AG29">
+        <v>0.71256364591911547</v>
+      </c>
+      <c r="AH29">
+        <v>-0.44761863553923142</v>
+      </c>
+      <c r="AI29">
+        <v>-0.40142529286127582</v>
+      </c>
+      <c r="AJ29">
+        <v>1.0156148251505639E-2</v>
+      </c>
+      <c r="AK29">
+        <v>0.71869627754185761</v>
+      </c>
     </row>
-    <row r="30" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>90</v>
+        <v>65</v>
       </c>
       <c r="B30">
         <v>156</v>
@@ -3696,10 +4152,25 @@
         <f t="shared" si="1"/>
         <v>115</v>
       </c>
+      <c r="AG30">
+        <v>-1.1820550322387831</v>
+      </c>
+      <c r="AH30">
+        <v>-0.73386681267922171</v>
+      </c>
+      <c r="AI30">
+        <v>1.6746602690182271</v>
+      </c>
+      <c r="AJ30">
+        <v>-4.6830942201214913E-2</v>
+      </c>
+      <c r="AK30">
+        <v>0.6728527929803918</v>
+      </c>
     </row>
-    <row r="31" spans="1:31" ht="19" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:37" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>122</v>
+        <v>66</v>
       </c>
       <c r="B31">
         <v>452</v>
@@ -3790,10 +4261,25 @@
       <c r="AD31" s="3">
         <v>45.3</v>
       </c>
+      <c r="AG31">
+        <v>1.986926802088252</v>
+      </c>
+      <c r="AH31">
+        <v>1.3649561464928011</v>
+      </c>
+      <c r="AI31">
+        <v>0.18959285363651171</v>
+      </c>
+      <c r="AJ31">
+        <v>1.0051042274821651</v>
+      </c>
+      <c r="AK31">
+        <v>0.52549873546139469</v>
+      </c>
     </row>
-    <row r="32" spans="1:31" ht="19" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:37" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B32">
         <v>570</v>
@@ -3887,10 +4373,25 @@
       <c r="AE32">
         <v>2.08</v>
       </c>
+      <c r="AG32">
+        <v>1.8332414620590869</v>
+      </c>
+      <c r="AH32">
+        <v>1.490538402828673</v>
+      </c>
+      <c r="AI32">
+        <v>-0.21556027575576381</v>
+      </c>
+      <c r="AJ32">
+        <v>1.75378268294482</v>
+      </c>
+      <c r="AK32">
+        <v>0.5016798604103786</v>
+      </c>
     </row>
-    <row r="33" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>137</v>
+        <v>68</v>
       </c>
       <c r="B33">
         <v>238</v>
@@ -3978,10 +4479,25 @@
         <f t="shared" si="1"/>
         <v>6</v>
       </c>
+      <c r="AG33">
+        <v>-0.28790289314419548</v>
+      </c>
+      <c r="AH33">
+        <v>-1.0008985439854321</v>
+      </c>
+      <c r="AI33">
+        <v>-1.365966907945666</v>
+      </c>
+      <c r="AJ33">
+        <v>-1.329683188933884</v>
+      </c>
+      <c r="AK33">
+        <v>0.49499386039605853</v>
+      </c>
     </row>
-    <row r="34" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="B34">
         <v>112</v>
@@ -4072,10 +4588,25 @@
       <c r="AE34">
         <v>2.33</v>
       </c>
+      <c r="AG34">
+        <v>-1.272662449000368</v>
+      </c>
+      <c r="AH34">
+        <v>1.620378399308861</v>
+      </c>
+      <c r="AI34">
+        <v>0.24920859710933349</v>
+      </c>
+      <c r="AJ34">
+        <v>1.451115435413151</v>
+      </c>
+      <c r="AK34">
+        <v>0.48685922704530182</v>
+      </c>
     </row>
-    <row r="35" spans="1:31" ht="19" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:37" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>36</v>
+        <v>70</v>
       </c>
       <c r="B35">
         <v>572</v>
@@ -4166,10 +4697,25 @@
       <c r="AD35" s="3">
         <v>45.3</v>
       </c>
+      <c r="AG35">
+        <v>1.6686408846144289</v>
+      </c>
+      <c r="AH35">
+        <v>0.18275765359209409</v>
+      </c>
+      <c r="AI35">
+        <v>-4.2472230825069332E-2</v>
+      </c>
+      <c r="AJ35">
+        <v>-0.57128356411196524</v>
+      </c>
+      <c r="AK35">
+        <v>0.43398411026538602</v>
+      </c>
     </row>
-    <row r="36" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>117</v>
+        <v>71</v>
       </c>
       <c r="B36">
         <v>356</v>
@@ -4260,10 +4806,25 @@
       <c r="AD36">
         <v>54.4</v>
       </c>
+      <c r="AG36">
+        <v>9.1639631647057376E-3</v>
+      </c>
+      <c r="AH36">
+        <v>-0.65396483090236346</v>
+      </c>
+      <c r="AI36">
+        <v>-0.99717158453104593</v>
+      </c>
+      <c r="AJ36">
+        <v>-1.140083282728404</v>
+      </c>
+      <c r="AK36">
+        <v>0.43398411026538602</v>
+      </c>
     </row>
-    <row r="37" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>54</v>
+        <v>72</v>
       </c>
       <c r="B37">
         <v>396</v>
@@ -4351,10 +4912,25 @@
         <f t="shared" si="3"/>
         <v>142</v>
       </c>
+      <c r="AG37">
+        <v>0.44150358729683842</v>
+      </c>
+      <c r="AH37">
+        <v>-0.27292482209315971</v>
+      </c>
+      <c r="AI37">
+        <v>-0.2595809377018069</v>
+      </c>
+      <c r="AJ37">
+        <v>-0.25961248541802628</v>
+      </c>
+      <c r="AK37">
+        <v>0.40640436020631471</v>
+      </c>
     </row>
-    <row r="38" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="B38">
         <v>207</v>
@@ -4442,10 +5018,25 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
+      <c r="AG38">
+        <v>-1.2519335618303979</v>
+      </c>
+      <c r="AH38">
+        <v>-0.70821988789813739</v>
+      </c>
+      <c r="AI38">
+        <v>0.97222530447253119</v>
+      </c>
+      <c r="AJ38">
+        <v>-0.91533802805556708</v>
+      </c>
+      <c r="AK38">
+        <v>0.39827108579865039</v>
+      </c>
     </row>
-    <row r="39" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>115</v>
+        <v>74</v>
       </c>
       <c r="B39">
         <v>236</v>
@@ -4533,10 +5124,25 @@
         <f t="shared" si="3"/>
         <v>75</v>
       </c>
+      <c r="AG39">
+        <v>-0.98162078107637352</v>
+      </c>
+      <c r="AH39">
+        <v>-0.59377454412026753</v>
+      </c>
+      <c r="AI39">
+        <v>0.26415206596392571</v>
+      </c>
+      <c r="AJ39">
+        <v>1.65783533314942</v>
+      </c>
+      <c r="AK39">
+        <v>0.37142980949849402</v>
+      </c>
     </row>
-    <row r="40" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>41</v>
+        <v>75</v>
       </c>
       <c r="B40">
         <v>196</v>
@@ -4624,10 +5230,25 @@
         <f t="shared" si="3"/>
         <v>42</v>
       </c>
+      <c r="AG40">
+        <v>-0.99192340527438061</v>
+      </c>
+      <c r="AH40">
+        <v>-0.80795145221730824</v>
+      </c>
+      <c r="AI40">
+        <v>-0.29826576183620751</v>
+      </c>
+      <c r="AJ40">
+        <v>1.407450002468859</v>
+      </c>
+      <c r="AK40">
+        <v>0.3674280192137433</v>
+      </c>
     </row>
-    <row r="41" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>113</v>
+        <v>76</v>
       </c>
       <c r="B41">
         <v>165</v>
@@ -4715,10 +5336,25 @@
         <f t="shared" si="3"/>
         <v>5</v>
       </c>
+      <c r="AG41">
+        <v>-1.3878185378396519</v>
+      </c>
+      <c r="AH41">
+        <v>-1.180034252047931</v>
+      </c>
+      <c r="AI41">
+        <v>-0.98298714901509909</v>
+      </c>
+      <c r="AJ41">
+        <v>0.97079567302593572</v>
+      </c>
+      <c r="AK41">
+        <v>0.33230119338093173</v>
+      </c>
     </row>
-    <row r="42" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>61</v>
+        <v>77</v>
       </c>
       <c r="B42">
         <v>542</v>
@@ -4812,10 +5448,25 @@
       <c r="AE42">
         <v>1.93</v>
       </c>
+      <c r="AG42">
+        <v>2.142844688664022</v>
+      </c>
+      <c r="AH42">
+        <v>2.5695360127391389</v>
+      </c>
+      <c r="AI42">
+        <v>-8.1551798062881584E-2</v>
+      </c>
+      <c r="AJ42">
+        <v>0.53481311947446375</v>
+      </c>
+      <c r="AK42">
+        <v>0.28474487533035631</v>
+      </c>
     </row>
-    <row r="43" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>116</v>
+        <v>78</v>
       </c>
       <c r="B43">
         <v>406</v>
@@ -4906,10 +5557,25 @@
       <c r="AD43">
         <v>46.1</v>
       </c>
+      <c r="AG43">
+        <v>1.5073028505845949</v>
+      </c>
+      <c r="AH43">
+        <v>1.0325994801779299</v>
+      </c>
+      <c r="AI43">
+        <v>4.0795343812363077E-2</v>
+      </c>
+      <c r="AJ43">
+        <v>-0.84755771315423534</v>
+      </c>
+      <c r="AK43">
+        <v>0.27710189564365673</v>
+      </c>
     </row>
-    <row r="44" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>133</v>
+        <v>79</v>
       </c>
       <c r="B44">
         <v>258</v>
@@ -4997,10 +5663,25 @@
         <f t="shared" si="3"/>
         <v>84</v>
       </c>
+      <c r="AG44">
+        <v>-0.66228852027322105</v>
+      </c>
+      <c r="AH44">
+        <v>-0.35791100160746492</v>
+      </c>
+      <c r="AI44">
+        <v>-2.747199289540251E-2</v>
+      </c>
+      <c r="AJ44">
+        <v>-1.799267614166085</v>
+      </c>
+      <c r="AK44">
+        <v>0.2158533597981869</v>
+      </c>
     </row>
-    <row r="45" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>160</v>
+        <v>80</v>
       </c>
       <c r="B45">
         <v>333</v>
@@ -5088,10 +5769,25 @@
         <f t="shared" si="3"/>
         <v>142</v>
       </c>
+      <c r="AG45">
+        <v>0.22009074358466241</v>
+      </c>
+      <c r="AH45">
+        <v>-0.26745222720019313</v>
+      </c>
+      <c r="AI45">
+        <v>-0.59392834629198399</v>
+      </c>
+      <c r="AJ45">
+        <v>-0.55749448002429425</v>
+      </c>
+      <c r="AK45">
+        <v>0.15666706421687471</v>
+      </c>
     </row>
-    <row r="46" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>145</v>
+        <v>81</v>
       </c>
       <c r="B46">
         <v>73</v>
@@ -5179,10 +5875,25 @@
         <f t="shared" si="3"/>
         <v>4</v>
       </c>
+      <c r="AG46">
+        <v>-6.1901599443673558E-2</v>
+      </c>
+      <c r="AH46">
+        <v>0.96335850802899814</v>
+      </c>
+      <c r="AI46">
+        <v>-0.47234747044101039</v>
+      </c>
+      <c r="AJ46">
+        <v>0.8507157324291319</v>
+      </c>
+      <c r="AK46">
+        <v>9.0804265780353083E-2</v>
+      </c>
     </row>
-    <row r="47" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>49</v>
+        <v>82</v>
       </c>
       <c r="B47">
         <v>172</v>
@@ -5270,10 +5981,25 @@
         <f t="shared" si="3"/>
         <v>102</v>
       </c>
+      <c r="AG47">
+        <v>-1.156695401788977</v>
+      </c>
+      <c r="AH47">
+        <v>-0.75727964987195362</v>
+      </c>
+      <c r="AI47">
+        <v>0.39123433891222792</v>
+      </c>
+      <c r="AJ47">
+        <v>-0.90545339879912323</v>
+      </c>
+      <c r="AK47">
+        <v>9.0804265780353083E-2</v>
+      </c>
     </row>
-    <row r="48" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>68</v>
+        <v>83</v>
       </c>
       <c r="B48">
         <v>324</v>
@@ -5361,10 +6087,25 @@
         <f t="shared" si="3"/>
         <v>122</v>
       </c>
+      <c r="AG48">
+        <v>-0.20349493121366599</v>
+      </c>
+      <c r="AH48">
+        <v>-0.53723184038264882</v>
+      </c>
+      <c r="AI48">
+        <v>-0.78407518119844855</v>
+      </c>
+      <c r="AJ48">
+        <v>-0.54701477611766436</v>
+      </c>
+      <c r="AK48">
+        <v>8.5008339517939457E-2</v>
+      </c>
     </row>
-    <row r="49" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>108</v>
+        <v>84</v>
       </c>
       <c r="B49">
         <v>253</v>
@@ -5452,10 +6193,25 @@
         <f t="shared" si="3"/>
         <v>121</v>
       </c>
+      <c r="AG49">
+        <v>-0.67417517038493591</v>
+      </c>
+      <c r="AH49">
+        <v>-1.1584926162682629</v>
+      </c>
+      <c r="AI49">
+        <v>-1.0526198324570211</v>
+      </c>
+      <c r="AJ49">
+        <v>-0.71032349532931749</v>
+      </c>
+      <c r="AK49">
+        <v>4.2504880260237722E-2</v>
+      </c>
     </row>
-    <row r="50" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>154</v>
+        <v>85</v>
       </c>
       <c r="B50">
         <v>389</v>
@@ -5543,10 +6299,25 @@
         <f t="shared" si="3"/>
         <v>82</v>
       </c>
+      <c r="AG50">
+        <v>0.61429457259313158</v>
+      </c>
+      <c r="AH50">
+        <v>0.23917939931840751</v>
+      </c>
+      <c r="AI50">
+        <v>0.19708869354331399</v>
+      </c>
+      <c r="AJ50">
+        <v>0.66000053265773839</v>
+      </c>
+      <c r="AK50">
+        <v>1.4093477013110339E-2</v>
+      </c>
     </row>
-    <row r="51" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>155</v>
+        <v>86</v>
       </c>
       <c r="B51">
         <v>267</v>
@@ -5634,10 +6405,25 @@
         <f t="shared" si="3"/>
         <v>64</v>
       </c>
+      <c r="AG51">
+        <v>-0.61916150784466151</v>
+      </c>
+      <c r="AH51">
+        <v>-6.1033604250061137E-2</v>
+      </c>
+      <c r="AI51">
+        <v>0.38479770430835281</v>
+      </c>
+      <c r="AJ51">
+        <v>-0.52209007493432757</v>
+      </c>
+      <c r="AK51">
+        <v>8.5647715163725113E-3</v>
+      </c>
     </row>
-    <row r="52" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>64</v>
+        <v>87</v>
       </c>
       <c r="B52">
         <v>314</v>
@@ -5728,10 +6514,25 @@
       <c r="AF52">
         <v>39.5</v>
       </c>
+      <c r="AG52">
+        <v>-0.43413149224107689</v>
+      </c>
+      <c r="AH52">
+        <v>-0.97538871214108835</v>
+      </c>
+      <c r="AI52">
+        <v>-0.7323954549000371</v>
+      </c>
+      <c r="AJ52">
+        <v>-1.385983986785503E-2</v>
+      </c>
+      <c r="AK52">
+        <v>3.865371844144698E-3</v>
+      </c>
     </row>
-    <row r="53" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="B53">
         <v>176</v>
@@ -5819,10 +6620,25 @@
         <f t="shared" si="3"/>
         <v>62</v>
       </c>
+      <c r="AG53">
+        <v>0.2102328599964442</v>
+      </c>
+      <c r="AH53">
+        <v>0.51744664738987811</v>
+      </c>
+      <c r="AI53">
+        <v>1.08794043631315</v>
+      </c>
+      <c r="AJ53">
+        <v>-0.16824833492088889</v>
+      </c>
+      <c r="AK53">
+        <v>-2.0974312137629209E-2</v>
+      </c>
     </row>
-    <row r="54" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>105</v>
+        <v>89</v>
       </c>
       <c r="B54">
         <v>365</v>
@@ -5913,10 +6729,25 @@
       <c r="AD54">
         <v>50.1</v>
       </c>
+      <c r="AG54">
+        <v>0.50318893893859928</v>
+      </c>
+      <c r="AH54">
+        <v>0.9780459869696807</v>
+      </c>
+      <c r="AI54">
+        <v>0.72099525666147946</v>
+      </c>
+      <c r="AJ54">
+        <v>1.276453703635982</v>
+      </c>
+      <c r="AK54">
+        <v>-5.4093890779993777E-2</v>
+      </c>
     </row>
-    <row r="55" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>39</v>
+        <v>90</v>
       </c>
       <c r="B55">
         <v>172</v>
@@ -6004,10 +6835,25 @@
         <f t="shared" si="3"/>
         <v>83</v>
       </c>
+      <c r="AG55">
+        <v>0.62173630824306048</v>
+      </c>
+      <c r="AH55">
+        <v>0.46574672151867641</v>
+      </c>
+      <c r="AI55">
+        <v>0.69161062042639843</v>
+      </c>
+      <c r="AJ55">
+        <v>0.77866776807104898</v>
+      </c>
+      <c r="AK55">
+        <v>-5.4093890779993777E-2</v>
+      </c>
     </row>
-    <row r="56" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>119</v>
+        <v>91</v>
       </c>
       <c r="B56">
         <v>434</v>
@@ -6095,10 +6941,25 @@
         <f t="shared" si="3"/>
         <v>151</v>
       </c>
+      <c r="AG56">
+        <v>0.79365948312987844</v>
+      </c>
+      <c r="AH56">
+        <v>0.71562969656282061</v>
+      </c>
+      <c r="AI56">
+        <v>-0.73517671676590957</v>
+      </c>
+      <c r="AJ56">
+        <v>-0.230003732942102</v>
+      </c>
+      <c r="AK56">
+        <v>-5.4093890779993777E-2</v>
+      </c>
     </row>
-    <row r="57" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>141</v>
+        <v>92</v>
       </c>
       <c r="B57">
         <v>221</v>
@@ -6186,10 +7047,25 @@
         <f t="shared" si="3"/>
         <v>18</v>
       </c>
+      <c r="AG57">
+        <v>-0.42161956307141579</v>
+      </c>
+      <c r="AH57">
+        <v>-0.4353091293794214</v>
+      </c>
+      <c r="AI57">
+        <v>-1.1921321237502309</v>
+      </c>
+      <c r="AJ57">
+        <v>-0.230003732942102</v>
+      </c>
+      <c r="AK57">
+        <v>-9.5493364082950546E-2</v>
+      </c>
     </row>
-    <row r="58" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>65</v>
+        <v>93</v>
       </c>
       <c r="B58">
         <v>215</v>
@@ -6277,10 +7153,25 @@
         <f t="shared" si="3"/>
         <v>14</v>
       </c>
+      <c r="AG58">
+        <v>-1.176068296233771</v>
+      </c>
+      <c r="AH58">
+        <v>-1.1560991011816339</v>
+      </c>
+      <c r="AI58">
+        <v>-0.87853812385221763</v>
+      </c>
+      <c r="AJ58">
+        <v>-1.217327688960266</v>
+      </c>
+      <c r="AK58">
+        <v>-9.7026677908986114E-2</v>
+      </c>
     </row>
-    <row r="59" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>111</v>
+        <v>94</v>
       </c>
       <c r="B59">
         <v>378</v>
@@ -6368,10 +7259,25 @@
         <f t="shared" si="3"/>
         <v>219</v>
       </c>
+      <c r="AG59">
+        <v>0.38269776160265861</v>
+      </c>
+      <c r="AH59">
+        <v>-5.9262384863533427E-2</v>
+      </c>
+      <c r="AI59">
+        <v>-0.48537399285361449</v>
+      </c>
+      <c r="AJ59">
+        <v>1.01815114255707</v>
+      </c>
+      <c r="AK59">
+        <v>-0.13572665503934489</v>
+      </c>
     </row>
-    <row r="60" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>86</v>
+        <v>95</v>
       </c>
       <c r="B60">
         <v>125</v>
@@ -6462,10 +7368,25 @@
       <c r="AE60">
         <v>3.15</v>
       </c>
+      <c r="AG60">
+        <v>-2.270527812513793E-2</v>
+      </c>
+      <c r="AH60">
+        <v>3.2862648996031578</v>
+      </c>
+      <c r="AI60">
+        <v>0.93964861046461445</v>
+      </c>
+      <c r="AJ60">
+        <v>1.7713286103379611</v>
+      </c>
+      <c r="AK60">
+        <v>-0.18289225216696961</v>
+      </c>
     </row>
-    <row r="61" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>85</v>
+        <v>96</v>
       </c>
       <c r="B61">
         <v>125</v>
@@ -6553,10 +7474,25 @@
         <f t="shared" si="3"/>
         <v>84</v>
       </c>
+      <c r="AG61">
+        <v>-2.270527812513793E-2</v>
+      </c>
+      <c r="AH61">
+        <v>-4.5508100985435833E-2</v>
+      </c>
+      <c r="AI61">
+        <v>-0.50594218613667419</v>
+      </c>
+      <c r="AJ61">
+        <v>-0.47016361413570962</v>
+      </c>
+      <c r="AK61">
+        <v>-0.18289225216696961</v>
+      </c>
     </row>
-    <row r="62" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>129</v>
+        <v>97</v>
       </c>
       <c r="B62">
         <v>285</v>
@@ -6647,10 +7583,25 @@
       <c r="AD62">
         <v>52.5</v>
       </c>
+      <c r="AG62">
+        <v>2.1109343546581818E-3</v>
+      </c>
+      <c r="AH62">
+        <v>-0.33178820052724822</v>
+      </c>
+      <c r="AI62">
+        <v>-1.00426380228902</v>
+      </c>
+      <c r="AJ62">
+        <v>-1.541040461425238</v>
+      </c>
+      <c r="AK62">
+        <v>-0.18711514926162409</v>
+      </c>
     </row>
-    <row r="63" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>125</v>
+        <v>98</v>
       </c>
       <c r="B63">
         <v>213</v>
@@ -6738,10 +7689,25 @@
         <f t="shared" si="3"/>
         <v>104</v>
       </c>
+      <c r="AG63">
+        <v>-0.89695020554626759</v>
+      </c>
+      <c r="AH63">
+        <v>-1.0153040960857671</v>
+      </c>
+      <c r="AI63">
+        <v>-1.110647068658621</v>
+      </c>
+      <c r="AJ63">
+        <v>-0.86572106551341621</v>
+      </c>
+      <c r="AK63">
+        <v>-0.19046862636620299</v>
+      </c>
     </row>
-    <row r="64" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>123</v>
+        <v>99</v>
       </c>
       <c r="B64">
         <v>218</v>
@@ -6829,10 +7795,25 @@
         <f t="shared" si="3"/>
         <v>146</v>
       </c>
+      <c r="AG64">
+        <v>-0.18013933009696609</v>
+      </c>
+      <c r="AH64">
+        <v>-0.53723184038264882</v>
+      </c>
+      <c r="AI64">
+        <v>-0.85532722937157701</v>
+      </c>
+      <c r="AJ64">
+        <v>-0.3164612901718008</v>
+      </c>
+      <c r="AK64">
+        <v>-0.23956353117723839</v>
+      </c>
     </row>
-    <row r="65" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>45</v>
+        <v>100</v>
       </c>
       <c r="B65">
         <v>403</v>
@@ -6920,10 +7901,25 @@
         <f t="shared" si="3"/>
         <v>232</v>
       </c>
+      <c r="AG65">
+        <v>0.45393367859830258</v>
+      </c>
+      <c r="AH65">
+        <v>0.42103327211655522</v>
+      </c>
+      <c r="AI65">
+        <v>1.9707992675643291</v>
+      </c>
+      <c r="AJ65">
+        <v>0.8799243666283546</v>
+      </c>
+      <c r="AK65">
+        <v>-0.27339920881727658</v>
+      </c>
     </row>
-    <row r="66" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>136</v>
+        <v>101</v>
       </c>
       <c r="B66">
         <v>597</v>
@@ -7014,10 +8010,25 @@
       <c r="AD66" s="2">
         <v>46.6</v>
       </c>
+      <c r="AG66">
+        <v>2.4768217402237189</v>
+      </c>
+      <c r="AH66">
+        <v>1.031359343363321</v>
+      </c>
+      <c r="AI66">
+        <v>0.25713778466482989</v>
+      </c>
+      <c r="AJ66">
+        <v>0.70554446096135404</v>
+      </c>
+      <c r="AK66">
+        <v>-0.27901043230650341</v>
+      </c>
     </row>
-    <row r="67" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>53</v>
+        <v>102</v>
       </c>
       <c r="B67">
         <v>25</v>
@@ -7105,8 +8116,23 @@
         <f t="shared" si="5"/>
         <v>11</v>
       </c>
+      <c r="AG67">
+        <v>-1.752749805288087</v>
+      </c>
+      <c r="AH67">
+        <v>-1.447150535715809</v>
+      </c>
+      <c r="AI67">
+        <v>-1.5361801341370289</v>
+      </c>
+      <c r="AJ67">
+        <v>-0.66229151909059547</v>
+      </c>
+      <c r="AK67">
+        <v>-0.28593094127654978</v>
+      </c>
     </row>
-    <row r="68" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>103</v>
       </c>
@@ -7199,10 +8225,25 @@
       <c r="AE68">
         <v>2.62</v>
       </c>
+      <c r="AG68">
+        <v>0.88556809863541008</v>
+      </c>
+      <c r="AH68">
+        <v>1.620378399308861</v>
+      </c>
+      <c r="AI68">
+        <v>0.99722602312976882</v>
+      </c>
+      <c r="AJ68">
+        <v>2.571861547649986</v>
+      </c>
+      <c r="AK68">
+        <v>-0.3116906135539449</v>
+      </c>
     </row>
-    <row r="69" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>127</v>
+        <v>104</v>
       </c>
       <c r="B69">
         <v>138</v>
@@ -7290,10 +8331,25 @@
         <f t="shared" si="5"/>
         <v>78</v>
       </c>
+      <c r="AG69">
+        <v>-1.011499344314813</v>
+      </c>
+      <c r="AH69">
+        <v>-0.30095217916702632</v>
+      </c>
+      <c r="AI69">
+        <v>-1.110647068658621</v>
+      </c>
+      <c r="AJ69">
+        <v>0.36784107768879348</v>
+      </c>
+      <c r="AK69">
+        <v>-0.32539256689298462</v>
+      </c>
     </row>
-    <row r="70" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>40</v>
+        <v>105</v>
       </c>
       <c r="B70">
         <v>448</v>
@@ -7387,10 +8443,25 @@
       <c r="AF70">
         <v>38</v>
       </c>
+      <c r="AG70">
+        <v>1.4262070133738309</v>
+      </c>
+      <c r="AH70">
+        <v>1.4480453130715201</v>
+      </c>
+      <c r="AI70">
+        <v>0.38605543750681148</v>
+      </c>
+      <c r="AJ70">
+        <v>0.90217856411347574</v>
+      </c>
+      <c r="AK70">
+        <v>-0.33009037946636949</v>
+      </c>
     </row>
-    <row r="71" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>40</v>
+        <v>105</v>
       </c>
       <c r="B71">
         <v>129</v>
@@ -7478,10 +8549,25 @@
         <f t="shared" si="5"/>
         <v>68</v>
       </c>
+      <c r="AG71">
+        <v>0.4125090482392913</v>
+      </c>
+      <c r="AH71">
+        <v>-0.16757737040355231</v>
+      </c>
+      <c r="AI71">
+        <v>0.87517390357394653</v>
+      </c>
+      <c r="AJ71">
+        <v>1.9314351978003661</v>
+      </c>
+      <c r="AK71">
+        <v>-0.34389020390068847</v>
+      </c>
     </row>
-    <row r="72" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="B72">
         <v>287</v>
@@ -7572,10 +8658,25 @@
       <c r="AD72">
         <v>55.7</v>
       </c>
+      <c r="AG72">
+        <v>0.26653654125991749</v>
+      </c>
+      <c r="AH72">
+        <v>-0.24143440736241281</v>
+      </c>
+      <c r="AI72">
+        <v>-0.83709009799393108</v>
+      </c>
+      <c r="AJ72">
+        <v>1.7770467027473329</v>
+      </c>
+      <c r="AK72">
+        <v>-0.34389020390068847</v>
+      </c>
     </row>
-    <row r="73" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>46</v>
+        <v>107</v>
       </c>
       <c r="B73">
         <v>231</v>
@@ -7663,10 +8764,25 @@
         <f t="shared" si="5"/>
         <v>89</v>
       </c>
+      <c r="AG73">
+        <v>8.4070907535700248E-2</v>
+      </c>
+      <c r="AH73">
+        <v>-3.8327555725546067E-2</v>
+      </c>
+      <c r="AI73">
+        <v>0.51411554498620748</v>
+      </c>
+      <c r="AJ73">
+        <v>0.8507157324291319</v>
+      </c>
+      <c r="AK73">
+        <v>-0.34389020390068847</v>
+      </c>
     </row>
-    <row r="74" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>151</v>
+        <v>108</v>
       </c>
       <c r="B74">
         <v>396</v>
@@ -7754,10 +8870,25 @@
         <f t="shared" si="5"/>
         <v>263</v>
       </c>
+      <c r="AG74">
+        <v>0.88691969592225617</v>
+      </c>
+      <c r="AH74">
+        <v>1.326873611810889</v>
+      </c>
+      <c r="AI74">
+        <v>0.57542734172752119</v>
+      </c>
+      <c r="AJ74">
+        <v>0.71562579925772762</v>
+      </c>
+      <c r="AK74">
+        <v>-0.34389020390068847</v>
+      </c>
     </row>
-    <row r="75" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>126</v>
+        <v>109</v>
       </c>
       <c r="B75">
         <v>287</v>
@@ -7845,10 +8976,25 @@
         <f t="shared" si="5"/>
         <v>167</v>
       </c>
+      <c r="AG75">
+        <v>-0.1075180078747279</v>
+      </c>
+      <c r="AH75">
+        <v>0.69678076525561128</v>
+      </c>
+      <c r="AI75">
+        <v>0.49252401523677369</v>
+      </c>
+      <c r="AJ75">
+        <v>-0.90545339879912323</v>
+      </c>
+      <c r="AK75">
+        <v>-0.34389020390068847</v>
+      </c>
     </row>
-    <row r="76" spans="1:32" ht="19" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:37" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>51</v>
+        <v>110</v>
       </c>
       <c r="B76">
         <v>482</v>
@@ -7942,10 +9088,25 @@
       <c r="AF76">
         <v>38.9</v>
       </c>
+      <c r="AG76">
+        <v>1.538266715701432</v>
+      </c>
+      <c r="AH76">
+        <v>0.43754676195256481</v>
+      </c>
+      <c r="AI76">
+        <v>-0.15945551053041759</v>
+      </c>
+      <c r="AJ76">
+        <v>-1.081479675355802</v>
+      </c>
+      <c r="AK76">
+        <v>-0.37023532327529712</v>
+      </c>
     </row>
-    <row r="77" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>132</v>
+        <v>111</v>
       </c>
       <c r="B77">
         <v>357</v>
@@ -8033,10 +9194,25 @@
         <f t="shared" si="5"/>
         <v>118</v>
       </c>
+      <c r="AG77">
+        <v>5.341668107003162E-2</v>
+      </c>
+      <c r="AH77">
+        <v>0.1658871514657019</v>
+      </c>
+      <c r="AI77">
+        <v>1.6249226379882811</v>
+      </c>
+      <c r="AJ77">
+        <v>-1.238675233955254</v>
+      </c>
+      <c r="AK77">
+        <v>-0.37866576147517178</v>
+      </c>
     </row>
-    <row r="78" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>98</v>
+        <v>112</v>
       </c>
       <c r="B78">
         <v>337</v>
@@ -8127,10 +9303,25 @@
       <c r="AF78">
         <v>43.6</v>
       </c>
+      <c r="AG78">
+        <v>-0.13680854381466809</v>
+      </c>
+      <c r="AH78">
+        <v>-0.77641202375521112</v>
+      </c>
+      <c r="AI78">
+        <v>-0.35414384114145248</v>
+      </c>
+      <c r="AJ78">
+        <v>0.1112760982277614</v>
+      </c>
+      <c r="AK78">
+        <v>-0.38964751649869322</v>
+      </c>
     </row>
-    <row r="79" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>52</v>
+        <v>113</v>
       </c>
       <c r="B79">
         <v>480</v>
@@ -8218,10 +9409,25 @@
         <f t="shared" si="5"/>
         <v>37</v>
       </c>
+      <c r="AG79">
+        <v>0.96182664029325071</v>
+      </c>
+      <c r="AH79">
+        <v>0.26438911549399341</v>
+      </c>
+      <c r="AI79">
+        <v>-0.24438332822043471</v>
+      </c>
+      <c r="AJ79">
+        <v>-2.4838454955266932E-3</v>
+      </c>
+      <c r="AK79">
+        <v>-0.38964751649869322</v>
+      </c>
     </row>
-    <row r="80" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>147</v>
+        <v>114</v>
       </c>
       <c r="B80">
         <v>358</v>
@@ -8312,10 +9518,25 @@
       <c r="AE80">
         <v>3.54</v>
       </c>
+      <c r="AG80">
+        <v>0.30355855389961373</v>
+      </c>
+      <c r="AH80">
+        <v>2.1448704009007691</v>
+      </c>
+      <c r="AI80">
+        <v>2.5160551939414422</v>
+      </c>
+      <c r="AJ80">
+        <v>1.492882371272908</v>
+      </c>
+      <c r="AK80">
+        <v>-0.40688940240518751</v>
+      </c>
     </row>
-    <row r="81" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>57</v>
+        <v>115</v>
       </c>
       <c r="B81">
         <v>196</v>
@@ -8403,10 +9624,25 @@
         <f t="shared" si="5"/>
         <v>117</v>
       </c>
+      <c r="AG81">
+        <v>-0.88005395711032519</v>
+      </c>
+      <c r="AH81">
+        <v>-1.103596189603949</v>
+      </c>
+      <c r="AI81">
+        <v>0.16595212777660071</v>
+      </c>
+      <c r="AJ81">
+        <v>-0.57862291531991961</v>
+      </c>
+      <c r="AK81">
+        <v>-0.42802461738734182</v>
+      </c>
     </row>
-    <row r="82" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>67</v>
+        <v>116</v>
       </c>
       <c r="B82">
         <v>331</v>
@@ -8494,10 +9730,25 @@
         <f t="shared" si="5"/>
         <v>195</v>
       </c>
+      <c r="AG82">
+        <v>-3.8209892723032532E-3</v>
+      </c>
+      <c r="AH82">
+        <v>0.26841320164408711</v>
+      </c>
+      <c r="AI82">
+        <v>0.49328525506768323</v>
+      </c>
+      <c r="AJ82">
+        <v>0.16575269099665921</v>
+      </c>
+      <c r="AK82">
+        <v>-0.42960460637300629</v>
+      </c>
     </row>
-    <row r="83" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="B83">
         <v>356</v>
@@ -8585,10 +9836,25 @@
         <f t="shared" si="5"/>
         <v>295</v>
       </c>
+      <c r="AG83">
+        <v>-0.1275892275843917</v>
+      </c>
+      <c r="AH83">
+        <v>-0.74273904572067795</v>
+      </c>
+      <c r="AI83">
+        <v>-0.95867097384490452</v>
+      </c>
+      <c r="AJ83">
+        <v>0.95878767896625539</v>
+      </c>
+      <c r="AK83">
+        <v>-0.43082909783689682</v>
+      </c>
     </row>
-    <row r="84" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>70</v>
+        <v>118</v>
       </c>
       <c r="B84">
         <v>89</v>
@@ -8676,10 +9942,25 @@
         <f t="shared" si="5"/>
         <v>44</v>
       </c>
+      <c r="AG84">
+        <v>-1.901039336187768</v>
+      </c>
+      <c r="AH84">
+        <v>-0.25066653698227032</v>
+      </c>
+      <c r="AI84">
+        <v>0.41145197324491289</v>
+      </c>
+      <c r="AJ84">
+        <v>0.90217856411347574</v>
+      </c>
+      <c r="AK84">
+        <v>-0.44048897494091999</v>
+      </c>
     </row>
-    <row r="85" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>47</v>
+        <v>60</v>
       </c>
       <c r="B85">
         <v>344</v>
@@ -8767,10 +10048,25 @@
         <f t="shared" si="5"/>
         <v>125</v>
       </c>
+      <c r="AG85">
+        <v>-0.24616936288368541</v>
+      </c>
+      <c r="AH85">
+        <v>-0.88802541147910297</v>
+      </c>
+      <c r="AI85">
+        <v>4.4371251925627277E-2</v>
+      </c>
+      <c r="AJ85">
+        <v>0.81068908556353003</v>
+      </c>
+      <c r="AK85">
+        <v>-0.44048897494091999</v>
+      </c>
     </row>
-    <row r="86" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>32</v>
+        <v>119</v>
       </c>
       <c r="B86">
         <v>237</v>
@@ -8858,10 +10154,25 @@
         <f t="shared" si="5"/>
         <v>175</v>
       </c>
+      <c r="AG86">
+        <v>-0.59694698079499375</v>
+      </c>
+      <c r="AH86">
+        <v>-0.34156750554702159</v>
+      </c>
+      <c r="AI86">
+        <v>2.2936174551686368</v>
+      </c>
+      <c r="AJ86">
+        <v>-0.79530314559782456</v>
+      </c>
+      <c r="AK86">
+        <v>-0.46426713396620761</v>
+      </c>
     </row>
-    <row r="87" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>96</v>
+        <v>120</v>
       </c>
       <c r="B87">
         <v>514</v>
@@ -8955,10 +10266,25 @@
       <c r="AE87">
         <v>1.93</v>
       </c>
+      <c r="AG87">
+        <v>2.6333764758540501</v>
+      </c>
+      <c r="AH87">
+        <v>1.946580312543829</v>
+      </c>
+      <c r="AI87">
+        <v>5.3311022208788209E-2</v>
+      </c>
+      <c r="AJ87">
+        <v>1.0051042274821651</v>
+      </c>
+      <c r="AK87">
+        <v>-0.46808862380955779</v>
+      </c>
     </row>
-    <row r="88" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>80</v>
+        <v>121</v>
       </c>
       <c r="B88">
         <v>248</v>
@@ -9046,10 +10372,25 @@
         <f t="shared" si="5"/>
         <v>145</v>
       </c>
+      <c r="AG88">
+        <v>-0.14010115675405219</v>
+      </c>
+      <c r="AH88">
+        <v>1.226474202194938</v>
+      </c>
+      <c r="AI88">
+        <v>7.1389224336954452E-2</v>
+      </c>
+      <c r="AJ88">
+        <v>0.8507157324291319</v>
+      </c>
+      <c r="AK88">
+        <v>-0.46808862380955779</v>
+      </c>
     </row>
-    <row r="89" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>143</v>
+        <v>122</v>
       </c>
       <c r="B89">
         <v>249</v>
@@ -9137,10 +10478,25 @@
         <f t="shared" si="5"/>
         <v>101</v>
       </c>
+      <c r="AG89">
+        <v>-0.78738495913116147</v>
+      </c>
+      <c r="AH89">
+        <v>-2.0232581670626221E-2</v>
+      </c>
+      <c r="AI89">
+        <v>0.76435800110560992</v>
+      </c>
+      <c r="AJ89">
+        <v>-0.77756826206352692</v>
+      </c>
+      <c r="AK89">
+        <v>-0.47140058167379378</v>
+      </c>
     </row>
-    <row r="90" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>48</v>
+        <v>123</v>
       </c>
       <c r="B90">
         <v>251</v>
@@ -9228,10 +10584,25 @@
         <f t="shared" si="5"/>
         <v>178</v>
       </c>
+      <c r="AG90">
+        <v>-0.77181455838669455</v>
+      </c>
+      <c r="AH90">
+        <v>-1.1783109211855569</v>
+      </c>
+      <c r="AI90">
+        <v>-0.75603618075994905</v>
+      </c>
+      <c r="AJ90">
+        <v>-0.89284500503645903</v>
+      </c>
+      <c r="AK90">
+        <v>-0.47140058167379378</v>
+      </c>
     </row>
-    <row r="91" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>79</v>
+        <v>124</v>
       </c>
       <c r="B91">
         <v>407</v>
@@ -9322,10 +10693,25 @@
       <c r="AF91">
         <v>36.4</v>
       </c>
+      <c r="AG91">
+        <v>0.40098490295144618</v>
+      </c>
+      <c r="AH91">
+        <v>0.18275765359209409</v>
+      </c>
+      <c r="AI91">
+        <v>-0.25958093770180768</v>
+      </c>
+      <c r="AJ91">
+        <v>-0.79880345155854071</v>
+      </c>
+      <c r="AK91">
+        <v>-0.48116214169470201</v>
+      </c>
     </row>
-    <row r="92" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>50</v>
+        <v>125</v>
       </c>
       <c r="B92">
         <v>99</v>
@@ -9413,10 +10799,25 @@
         <f t="shared" si="5"/>
         <v>55</v>
       </c>
+      <c r="AG92">
+        <v>-1.2437174732574501</v>
+      </c>
+      <c r="AH92">
+        <v>-0.26202915805286409</v>
+      </c>
+      <c r="AI92">
+        <v>1.336168057842221</v>
+      </c>
+      <c r="AJ92">
+        <v>1.3772200873535789</v>
+      </c>
+      <c r="AK92">
+        <v>-0.49993437250413902</v>
+      </c>
     </row>
-    <row r="93" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>34</v>
+        <v>126</v>
       </c>
       <c r="B93">
         <v>312</v>
@@ -9504,10 +10905,25 @@
         <f t="shared" si="5"/>
         <v>143</v>
       </c>
+      <c r="AG93">
+        <v>-0.1234185845278381</v>
+      </c>
+      <c r="AH93">
+        <v>1.1600028689319639</v>
+      </c>
+      <c r="AI93">
+        <v>0.92149042770765044</v>
+      </c>
+      <c r="AJ93">
+        <v>2.4254783819700729</v>
+      </c>
+      <c r="AK93">
+        <v>-0.51776799177310506</v>
+      </c>
     </row>
-    <row r="94" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>159</v>
+        <v>127</v>
       </c>
       <c r="B94">
         <v>278</v>
@@ -9595,10 +11011,25 @@
         <f t="shared" si="5"/>
         <v>80</v>
       </c>
+      <c r="AG94">
+        <v>1.3321358422093461</v>
+      </c>
+      <c r="AH94">
+        <v>0.67254642500348516</v>
+      </c>
+      <c r="AI94">
+        <v>-0.47234747044101039</v>
+      </c>
+      <c r="AJ94">
+        <v>-0.44614762601634872</v>
+      </c>
+      <c r="AK94">
+        <v>-0.51776799177310506</v>
+      </c>
     </row>
-    <row r="95" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>149</v>
+        <v>128</v>
       </c>
       <c r="B95">
         <v>224</v>
@@ -9686,10 +11117,25 @@
         <f t="shared" si="5"/>
         <v>139</v>
       </c>
+      <c r="AG95">
+        <v>-0.88376793275359844</v>
+      </c>
+      <c r="AH95">
+        <v>-1.1078242616879179</v>
+      </c>
+      <c r="AI95">
+        <v>-0.70751048031065644</v>
+      </c>
+      <c r="AJ95">
+        <v>-0.68664576056375004</v>
+      </c>
+      <c r="AK95">
+        <v>-0.5275639234842272</v>
+      </c>
     </row>
-    <row r="96" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>156</v>
+        <v>129</v>
       </c>
       <c r="B96">
         <v>274</v>
@@ -9777,10 +11223,25 @@
         <f t="shared" si="5"/>
         <v>151</v>
       </c>
+      <c r="AG96">
+        <v>-0.50387391224233347</v>
+      </c>
+      <c r="AH96">
+        <v>0.56483824610514777</v>
+      </c>
+      <c r="AI96">
+        <v>0.67065413566959631</v>
+      </c>
+      <c r="AJ96">
+        <v>1.331035494816347</v>
+      </c>
+      <c r="AK96">
+        <v>-0.53708774598115139</v>
+      </c>
     </row>
-    <row r="97" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>101</v>
+        <v>130</v>
       </c>
       <c r="B97">
         <v>238</v>
@@ -9871,10 +11332,25 @@
       <c r="AE97">
         <v>2.78</v>
       </c>
+      <c r="AG97">
+        <v>-0.48451555110169919</v>
+      </c>
+      <c r="AH97">
+        <v>1.7732545241968249</v>
+      </c>
+      <c r="AI97">
+        <v>2.9125746413190492</v>
+      </c>
+      <c r="AJ97">
+        <v>-2.083222351541127E-2</v>
+      </c>
+      <c r="AK97">
+        <v>-0.54020383536954597</v>
+      </c>
     </row>
-    <row r="98" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>56</v>
+        <v>131</v>
       </c>
       <c r="B98">
         <v>72</v>
@@ -9962,10 +11438,25 @@
         <f t="shared" ref="AC98:AC129" si="7">SUM(Z98,AA98)</f>
         <v>33</v>
       </c>
+      <c r="AG98">
+        <v>-0.72399118467154799</v>
+      </c>
+      <c r="AH98">
+        <v>-0.47223764785885169</v>
+      </c>
+      <c r="AI98">
+        <v>-0.53037470664261166</v>
+      </c>
+      <c r="AJ98">
+        <v>-0.74463204978554653</v>
+      </c>
+      <c r="AK98">
+        <v>-0.55088757041547021</v>
+      </c>
     </row>
-    <row r="99" spans="1:31" ht="19" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:37" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>91</v>
+        <v>132</v>
       </c>
       <c r="B99">
         <v>238</v>
@@ -10056,10 +11547,25 @@
       <c r="AD99" s="3">
         <v>42.1</v>
       </c>
+      <c r="AG99">
+        <v>1.6167822308191251</v>
+      </c>
+      <c r="AH99">
+        <v>0.86642114702049389</v>
+      </c>
+      <c r="AI99">
+        <v>-0.80669487903118753</v>
+      </c>
+      <c r="AJ99">
+        <v>3.0121546631716001</v>
+      </c>
+      <c r="AK99">
+        <v>-0.56123743874120924</v>
+      </c>
     </row>
-    <row r="100" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>146</v>
+        <v>133</v>
       </c>
       <c r="B100">
         <v>123</v>
@@ -10147,10 +11653,25 @@
         <f t="shared" si="7"/>
         <v>3</v>
       </c>
+      <c r="AG100">
+        <v>-1.055702795216038</v>
+      </c>
+      <c r="AH100">
+        <v>-1.221113650511483</v>
+      </c>
+      <c r="AI100">
+        <v>-1.208847006845946</v>
+      </c>
+      <c r="AJ100">
+        <v>-1.3861222307810961</v>
+      </c>
+      <c r="AK100">
+        <v>-0.56629202559796554</v>
+      </c>
     </row>
-    <row r="101" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>29</v>
+        <v>134</v>
       </c>
       <c r="B101">
         <v>195</v>
@@ -10238,10 +11759,25 @@
         <f t="shared" si="7"/>
         <v>54</v>
       </c>
+      <c r="AG101">
+        <v>-0.61740808433740157</v>
+      </c>
+      <c r="AH101">
+        <v>-0.96461789425125455</v>
+      </c>
+      <c r="AI101">
+        <v>-0.92827575488216119</v>
+      </c>
+      <c r="AJ101">
+        <v>-0.14995043921090009</v>
+      </c>
+      <c r="AK101">
+        <v>-0.5692873363278953</v>
+      </c>
     </row>
-    <row r="102" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>63</v>
+        <v>135</v>
       </c>
       <c r="B102">
         <v>147</v>
@@ -10329,10 +11865,25 @@
         <f t="shared" si="7"/>
         <v>135</v>
       </c>
+      <c r="AG102">
+        <v>-1.4448277010131889</v>
+      </c>
+      <c r="AH102">
+        <v>-1.0983689462563551</v>
+      </c>
+      <c r="AI102">
+        <v>1.4425513242118211</v>
+      </c>
+      <c r="AJ102">
+        <v>-1.1010313617487679</v>
+      </c>
+      <c r="AK102">
+        <v>-0.59043333595859271</v>
+      </c>
     </row>
-    <row r="103" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>131</v>
+        <v>136</v>
       </c>
       <c r="B103">
         <v>117</v>
@@ -10423,10 +11974,25 @@
       <c r="AE103">
         <v>2.34</v>
       </c>
+      <c r="AG103">
+        <v>0.24432333367610001</v>
+      </c>
+      <c r="AH103">
+        <v>3.3362165188023871</v>
+      </c>
+      <c r="AI103">
+        <v>1.1115811621730609</v>
+      </c>
+      <c r="AJ103">
+        <v>2.1193864091692758</v>
+      </c>
+      <c r="AK103">
+        <v>-0.60848683761958333</v>
+      </c>
     </row>
-    <row r="104" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>153</v>
+        <v>137</v>
       </c>
       <c r="B104">
         <v>173</v>
@@ -10514,10 +12080,25 @@
         <f t="shared" si="7"/>
         <v>96</v>
       </c>
+      <c r="AG104">
+        <v>-0.62146287619793961</v>
+      </c>
+      <c r="AH104">
+        <v>-0.91076380480208541</v>
+      </c>
+      <c r="AI104">
+        <v>-1.4085202144935061</v>
+      </c>
+      <c r="AJ104">
+        <v>0.8507157324291319</v>
+      </c>
+      <c r="AK104">
+        <v>-0.6336865170213829</v>
+      </c>
     </row>
-    <row r="105" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>128</v>
+        <v>138</v>
       </c>
       <c r="B105">
         <v>346</v>
@@ -10605,10 +12186,25 @@
         <f t="shared" si="7"/>
         <v>99</v>
       </c>
+      <c r="AG105">
+        <v>-0.1021862198762935</v>
+      </c>
+      <c r="AH105">
+        <v>-0.54609468481771206</v>
+      </c>
+      <c r="AI105">
+        <v>-0.67473514792464306</v>
+      </c>
+      <c r="AJ105">
+        <v>-0.14579182654953851</v>
+      </c>
+      <c r="AK105">
+        <v>-0.67132240184225223</v>
+      </c>
     </row>
-    <row r="106" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>135</v>
+        <v>139</v>
       </c>
       <c r="B106">
         <v>226</v>
@@ -10699,10 +12295,25 @@
       <c r="AE106">
         <v>4.5</v>
       </c>
+      <c r="AG106">
+        <v>-0.69575913936564671</v>
+      </c>
+      <c r="AH106">
+        <v>1.8775523895399699</v>
+      </c>
+      <c r="AI106">
+        <v>3.910643103986585</v>
+      </c>
+      <c r="AJ106">
+        <v>1.1998712520106081</v>
+      </c>
+      <c r="AK106">
+        <v>-0.67827056519379736</v>
+      </c>
     </row>
-    <row r="107" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
-        <v>124</v>
+        <v>140</v>
       </c>
       <c r="B107">
         <v>185</v>
@@ -10790,10 +12401,25 @@
         <f t="shared" si="7"/>
         <v>81</v>
       </c>
+      <c r="AG107">
+        <v>-0.7255358672850859</v>
+      </c>
+      <c r="AH107">
+        <v>0.95976823539905309</v>
+      </c>
+      <c r="AI107">
+        <v>-0.23594021184189551</v>
+      </c>
+      <c r="AJ107">
+        <v>0.65058249810112623</v>
+      </c>
+      <c r="AK107">
+        <v>-0.6980856977148705</v>
+      </c>
     </row>
-    <row r="108" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
-        <v>87</v>
+        <v>141</v>
       </c>
       <c r="B108">
         <v>192</v>
@@ -10881,10 +12507,25 @@
         <f t="shared" si="7"/>
         <v>100</v>
       </c>
+      <c r="AG108">
+        <v>-0.64984641922170727</v>
+      </c>
+      <c r="AH108">
+        <v>-1.0507844373699251</v>
+      </c>
+      <c r="AI108">
+        <v>-1.4297968677674271</v>
+      </c>
+      <c r="AJ108">
+        <v>0.33036932317631568</v>
+      </c>
+      <c r="AK108">
+        <v>-0.6980856977148705</v>
+      </c>
     </row>
-    <row r="109" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
-        <v>81</v>
+        <v>142</v>
       </c>
       <c r="B109">
         <v>319</v>
@@ -10972,10 +12613,25 @@
         <f t="shared" si="7"/>
         <v>171</v>
       </c>
+      <c r="AG109">
+        <v>1.323130856041654E-2</v>
+      </c>
+      <c r="AH109">
+        <v>-0.19418762636667111</v>
+      </c>
+      <c r="AI109">
+        <v>-0.68511400318021409</v>
+      </c>
+      <c r="AJ109">
+        <v>-0.230003732942102</v>
+      </c>
+      <c r="AK109">
+        <v>-0.70187388481448743</v>
+      </c>
     </row>
-    <row r="110" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
-        <v>162</v>
+        <v>143</v>
       </c>
       <c r="B110">
         <v>116</v>
@@ -11063,10 +12719,25 @@
         <f t="shared" si="7"/>
         <v>43</v>
       </c>
+      <c r="AG110">
+        <v>-1.073918309416527</v>
+      </c>
+      <c r="AH110">
+        <v>-1.0865120284191301</v>
+      </c>
+      <c r="AI110">
+        <v>0.8042517259942128</v>
+      </c>
+      <c r="AJ110">
+        <v>-1.3370822096638539</v>
+      </c>
+      <c r="AK110">
+        <v>-0.7043685446117961</v>
+      </c>
     </row>
-    <row r="111" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
-        <v>140</v>
+        <v>144</v>
       </c>
       <c r="B111">
         <v>71</v>
@@ -11154,10 +12825,25 @@
         <f t="shared" si="7"/>
         <v>32</v>
       </c>
+      <c r="AG111">
+        <v>0.23525671833576581</v>
+      </c>
+      <c r="AH111">
+        <v>-0.1029524630645494</v>
+      </c>
+      <c r="AI111">
+        <v>-0.60000739008453274</v>
+      </c>
+      <c r="AJ111">
+        <v>1.313881217588232</v>
+      </c>
+      <c r="AK111">
+        <v>-0.71648546362729559</v>
+      </c>
     </row>
-    <row r="112" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
-        <v>66</v>
+        <v>145</v>
       </c>
       <c r="B112">
         <v>295</v>
@@ -11245,10 +12931,25 @@
         <f t="shared" si="7"/>
         <v>132</v>
       </c>
+      <c r="AG112">
+        <v>0.34994940239098848</v>
+      </c>
+      <c r="AH112">
+        <v>-0.40761274051984869</v>
+      </c>
+      <c r="AI112">
+        <v>-0.2595809377018069</v>
+      </c>
+      <c r="AJ112">
+        <v>-1.6195001884194029</v>
+      </c>
+      <c r="AK112">
+        <v>-0.71648546362729559</v>
+      </c>
     </row>
-    <row r="113" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
-        <v>82</v>
+        <v>146</v>
       </c>
       <c r="B113">
         <v>190</v>
@@ -11336,10 +13037,25 @@
         <f t="shared" si="7"/>
         <v>128</v>
       </c>
+      <c r="AG113">
+        <v>-0.77959975875892829</v>
+      </c>
+      <c r="AH113">
+        <v>-0.32063636146961177</v>
+      </c>
+      <c r="AI113">
+        <v>1.7829777765945489</v>
+      </c>
+      <c r="AJ113">
+        <v>-1.1780032639695011</v>
+      </c>
+      <c r="AK113">
+        <v>-0.72520114221739163</v>
+      </c>
     </row>
-    <row r="114" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
-        <v>142</v>
+        <v>147</v>
       </c>
       <c r="B114">
         <v>324</v>
@@ -11427,10 +13143,25 @@
         <f t="shared" si="7"/>
         <v>67</v>
       </c>
+      <c r="AG114">
+        <v>0.48054708115340589</v>
+      </c>
+      <c r="AH114">
+        <v>0.79084286555623629</v>
+      </c>
+      <c r="AI114">
+        <v>-1.2771759724330299E-2</v>
+      </c>
+      <c r="AJ114">
+        <v>0.53932198816962373</v>
+      </c>
+      <c r="AK114">
+        <v>-0.74174615920198073</v>
+      </c>
     </row>
-    <row r="115" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
-        <v>66</v>
+        <v>145</v>
       </c>
       <c r="B115">
         <v>244</v>
@@ -11518,10 +13249,25 @@
         <f t="shared" si="7"/>
         <v>118</v>
       </c>
+      <c r="AG115">
+        <v>-0.82631096099232793</v>
+      </c>
+      <c r="AH115">
+        <v>0.1038472404202594</v>
+      </c>
+      <c r="AI115">
+        <v>1.953191002785911</v>
+      </c>
+      <c r="AJ115">
+        <v>-0.54701477611766436</v>
+      </c>
+      <c r="AK115">
+        <v>-0.74960504226966063</v>
+      </c>
     </row>
-    <row r="116" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
-        <v>44</v>
+        <v>148</v>
       </c>
       <c r="B116">
         <v>442</v>
@@ -11612,10 +13358,25 @@
       <c r="AF116">
         <v>38.9</v>
       </c>
+      <c r="AG116">
+        <v>0.6698816263345031</v>
+      </c>
+      <c r="AH116">
+        <v>1.4276374475960449</v>
+      </c>
+      <c r="AI116">
+        <v>0.53345795705340726</v>
+      </c>
+      <c r="AJ116">
+        <v>1.9314351978003661</v>
+      </c>
+      <c r="AK116">
+        <v>-0.7557060172827279</v>
+      </c>
     </row>
-    <row r="117" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="B117">
         <v>360</v>
@@ -11703,10 +13464,25 @@
         <f t="shared" si="7"/>
         <v>152</v>
       </c>
+      <c r="AG117">
+        <v>3.9895017265626893E-2</v>
+      </c>
+      <c r="AH117">
+        <v>-0.67437269637783814</v>
+      </c>
+      <c r="AI117">
+        <v>-0.27425449168382099</v>
+      </c>
+      <c r="AJ117">
+        <v>-2.4838454955266932E-3</v>
+      </c>
+      <c r="AK117">
+        <v>-0.7557060172827279</v>
+      </c>
     </row>
-    <row r="118" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
-        <v>144</v>
+        <v>150</v>
       </c>
       <c r="B118">
         <v>352</v>
@@ -11794,10 +13570,25 @@
         <f t="shared" si="7"/>
         <v>133</v>
       </c>
+      <c r="AG118">
+        <v>-2.1567090936214901E-2</v>
+      </c>
+      <c r="AH118">
+        <v>-0.63355696542688877</v>
+      </c>
+      <c r="AI118">
+        <v>-0.70751048031065644</v>
+      </c>
+      <c r="AJ118">
+        <v>-0.45752362038867761</v>
+      </c>
+      <c r="AK118">
+        <v>-0.7557060172827279</v>
+      </c>
     </row>
-    <row r="119" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
-        <v>60</v>
+        <v>151</v>
       </c>
       <c r="B119">
         <v>310</v>
@@ -11888,10 +13679,25 @@
       <c r="AF119">
         <v>39.200000000000003</v>
       </c>
+      <c r="AG119">
+        <v>-0.34424315899588359</v>
+      </c>
+      <c r="AH119">
+        <v>-0.83763562018163484</v>
+      </c>
+      <c r="AI119">
+        <v>-0.49598819630092172</v>
+      </c>
+      <c r="AJ119">
+        <v>-1.36760317017498</v>
+      </c>
+      <c r="AK119">
+        <v>-0.7557060172827279</v>
+      </c>
     </row>
-    <row r="120" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
-        <v>83</v>
+        <v>152</v>
       </c>
       <c r="B120">
         <v>208</v>
@@ -11979,10 +13785,25 @@
         <f t="shared" si="7"/>
         <v>68</v>
       </c>
+      <c r="AG120">
+        <v>-1.148638477702453</v>
+      </c>
+      <c r="AH120">
+        <v>-0.5058090282946972</v>
+      </c>
+      <c r="AI120">
+        <v>-0.52144743953467254</v>
+      </c>
+      <c r="AJ120">
+        <v>-3.3509284692786918E-2</v>
+      </c>
+      <c r="AK120">
+        <v>-0.76164852541233885</v>
+      </c>
     </row>
-    <row r="121" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
-        <v>27</v>
+        <v>153</v>
       </c>
       <c r="B121">
         <v>682</v>
@@ -12079,10 +13900,25 @@
       <c r="AF121">
         <v>38.200000000000003</v>
       </c>
+      <c r="AG121">
+        <v>2.3793950076664938</v>
+      </c>
+      <c r="AH121">
+        <v>2.7007742861044979</v>
+      </c>
+      <c r="AI121">
+        <v>0.71914511289852945</v>
+      </c>
+      <c r="AJ121">
+        <v>0.37963288854936311</v>
+      </c>
+      <c r="AK121">
+        <v>-0.7674386615386265</v>
+      </c>
     </row>
-    <row r="122" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
-        <v>93</v>
+        <v>154</v>
       </c>
       <c r="B122">
         <v>403</v>
@@ -12170,10 +14006,25 @@
         <f t="shared" si="7"/>
         <v>113</v>
       </c>
+      <c r="AG122">
+        <v>0.29086529242314663</v>
+      </c>
+      <c r="AH122">
+        <v>1.0901227493478109</v>
+      </c>
+      <c r="AI122">
+        <v>0.2421670051757181</v>
+      </c>
+      <c r="AJ122">
+        <v>-0.28542524398678049</v>
+      </c>
+      <c r="AK122">
+        <v>-0.7674386615386265</v>
+      </c>
     </row>
-    <row r="123" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
-        <v>97</v>
+        <v>155</v>
       </c>
       <c r="B123">
         <v>151</v>
@@ -12261,10 +14112,25 @@
         <f t="shared" si="7"/>
         <v>45</v>
       </c>
+      <c r="AG123">
+        <v>2.9331217418435071E-2</v>
+      </c>
+      <c r="AH123">
+        <v>-0.3937645460900624</v>
+      </c>
+      <c r="AI123">
+        <v>0.16595212777660071</v>
+      </c>
+      <c r="AJ123">
+        <v>4.0176133400706478E-2</v>
+      </c>
+      <c r="AK123">
+        <v>-0.77858467358173</v>
+      </c>
     </row>
-    <row r="124" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
-        <v>72</v>
+        <v>156</v>
       </c>
       <c r="B124">
         <v>363</v>
@@ -12352,10 +14218,25 @@
         <f t="shared" si="7"/>
         <v>220</v>
       </c>
+      <c r="AG124">
+        <v>-7.6498850141611147E-2</v>
+      </c>
+      <c r="AH124">
+        <v>-0.23866476847645551</v>
+      </c>
+      <c r="AI124">
+        <v>2.2723408018947171</v>
+      </c>
+      <c r="AJ124">
+        <v>-0.1219317864049785</v>
+      </c>
+      <c r="AK124">
+        <v>-0.77858467358173</v>
+      </c>
     </row>
-    <row r="125" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
-        <v>106</v>
+        <v>157</v>
       </c>
       <c r="B125">
         <v>293</v>
@@ -12443,10 +14324,25 @@
         <f t="shared" si="7"/>
         <v>137</v>
       </c>
+      <c r="AG125">
+        <v>-0.1337820006077596</v>
+      </c>
+      <c r="AH125">
+        <v>0.7195463576136687</v>
+      </c>
+      <c r="AI125">
+        <v>0.68267085014323747</v>
+      </c>
+      <c r="AJ125">
+        <v>-3.3509284692786918E-2</v>
+      </c>
+      <c r="AK125">
+        <v>-0.79175723326903436</v>
+      </c>
     </row>
-    <row r="126" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
-        <v>143</v>
+        <v>122</v>
       </c>
       <c r="B126">
         <v>498</v>
@@ -12537,10 +14433,25 @@
       <c r="AD126" s="2">
         <v>44.8</v>
       </c>
+      <c r="AG126">
+        <v>1.6140588631515991</v>
+      </c>
+      <c r="AH126">
+        <v>0.4989272709584025</v>
+      </c>
+      <c r="AI126">
+        <v>-0.40851751061924979</v>
+      </c>
+      <c r="AJ126">
+        <v>0.57650333076777349</v>
+      </c>
+      <c r="AK126">
+        <v>-0.79804860505998554</v>
+      </c>
     </row>
-    <row r="127" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
-        <v>118</v>
+        <v>158</v>
       </c>
       <c r="B127">
         <v>365</v>
@@ -12628,10 +14539,25 @@
         <f t="shared" si="7"/>
         <v>127</v>
       </c>
+      <c r="AG127">
+        <v>0.40821573921048587</v>
+      </c>
+      <c r="AH127">
+        <v>-0.46789311627303642</v>
+      </c>
+      <c r="AI127">
+        <v>-0.87853812385221763</v>
+      </c>
+      <c r="AJ127">
+        <v>-0.1028602664278392</v>
+      </c>
+      <c r="AK127">
+        <v>-0.80415493650414416</v>
+      </c>
     </row>
-    <row r="128" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
-        <v>152</v>
+        <v>159</v>
       </c>
       <c r="B128">
         <v>359</v>
@@ -12719,10 +14645,25 @@
         <f t="shared" si="7"/>
         <v>215</v>
       </c>
+      <c r="AG128">
+        <v>0.2686218627881945</v>
+      </c>
+      <c r="AH128">
+        <v>-0.50178046264239573</v>
+      </c>
+      <c r="AI128">
+        <v>0.1659521277766012</v>
+      </c>
+      <c r="AJ128">
+        <v>1.6844136057155119</v>
+      </c>
+      <c r="AK128">
+        <v>-0.8158441995543908</v>
+      </c>
     </row>
-    <row r="129" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
-        <v>28</v>
+        <v>160</v>
       </c>
       <c r="B129">
         <v>256</v>
@@ -12810,10 +14751,25 @@
         <f t="shared" si="7"/>
         <v>144</v>
       </c>
+      <c r="AG129">
+        <v>-0.73288855652552809</v>
+      </c>
+      <c r="AH129">
+        <v>-0.55791181073112972</v>
+      </c>
+      <c r="AI129">
+        <v>0.31914403134882752</v>
+      </c>
+      <c r="AJ129">
+        <v>-1.4692287199011169</v>
+      </c>
+      <c r="AK129">
+        <v>-0.84233986246828274</v>
+      </c>
     </row>
-    <row r="130" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
-        <v>110</v>
+        <v>161</v>
       </c>
       <c r="B130">
         <v>272</v>
@@ -12904,10 +14860,25 @@
       <c r="AF130">
         <v>34</v>
       </c>
+      <c r="AG130">
+        <v>-0.28254465807018853</v>
+      </c>
+      <c r="AH130">
+        <v>0.92309221961008181</v>
+      </c>
+      <c r="AI130">
+        <v>1.6678335353474509</v>
+      </c>
+      <c r="AJ130">
+        <v>-0.52927989258336672</v>
+      </c>
+      <c r="AK130">
+        <v>-0.89227399642138705</v>
+      </c>
     </row>
-    <row r="131" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
-        <v>35</v>
+        <v>162</v>
       </c>
       <c r="B131">
         <v>458</v>
@@ -12998,10 +14969,25 @@
       <c r="AD131">
         <v>47.3</v>
       </c>
+      <c r="AG131">
+        <v>1.3882791141244899</v>
+      </c>
+      <c r="AH131">
+        <v>1.6355058176686949E-2</v>
+      </c>
+      <c r="AI131">
+        <v>-0.40142529286127548</v>
+      </c>
+      <c r="AJ131">
+        <v>-0.66229151909059547</v>
+      </c>
+      <c r="AK131">
+        <v>-0.89227399642138705</v>
+      </c>
     </row>
-    <row r="132" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
-        <v>138</v>
+        <v>163</v>
       </c>
       <c r="B132">
         <v>184</v>
@@ -13092,10 +15078,25 @@
       <c r="AE132">
         <v>2.52</v>
       </c>
+      <c r="AG132">
+        <v>0.9787817046247933</v>
+      </c>
+      <c r="AH132">
+        <v>1.5015279950072471</v>
+      </c>
+      <c r="AI132">
+        <v>1.797162212110496</v>
+      </c>
+      <c r="AJ132">
+        <v>-1.497054140618721</v>
+      </c>
+      <c r="AK132">
+        <v>-0.97344771171461086</v>
+      </c>
     </row>
-    <row r="133" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
-        <v>75</v>
+        <v>164</v>
       </c>
       <c r="B133">
         <v>161</v>
@@ -13183,10 +15184,25 @@
         <f t="shared" si="9"/>
         <v>103</v>
       </c>
+      <c r="AG133">
+        <v>0.21179685114265229</v>
+      </c>
+      <c r="AH133">
+        <v>-0.3937645460900624</v>
+      </c>
+      <c r="AI133">
+        <v>0.16595212777660071</v>
+      </c>
+      <c r="AJ133">
+        <v>-1.040543331970528</v>
+      </c>
+      <c r="AK133">
+        <v>-0.99593190842225077</v>
+      </c>
     </row>
-    <row r="134" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
-        <v>30</v>
+        <v>165</v>
       </c>
       <c r="B134">
         <v>163</v>
@@ -13274,10 +15290,25 @@
         <f t="shared" si="9"/>
         <v>102</v>
       </c>
+      <c r="AG134">
+        <v>-1.3053912764358759</v>
+      </c>
+      <c r="AH134">
+        <v>-1.237264269492421</v>
+      </c>
+      <c r="AI134">
+        <v>0.16595212777660071</v>
+      </c>
+      <c r="AJ134">
+        <v>-1.617195882523089</v>
+      </c>
+      <c r="AK134">
+        <v>-1.005663874161379</v>
+      </c>
     </row>
-    <row r="135" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
-        <v>89</v>
+        <v>166</v>
       </c>
       <c r="B135">
         <v>396</v>
@@ -13365,10 +15396,25 @@
         <f t="shared" si="9"/>
         <v>201</v>
       </c>
+      <c r="AG135">
+        <v>0.35703949558712939</v>
+      </c>
+      <c r="AH135">
+        <v>0.47608670669291597</v>
+      </c>
+      <c r="AI135">
+        <v>4.7748498477042829E-2</v>
+      </c>
+      <c r="AJ135">
+        <v>-0.20118454719886841</v>
+      </c>
+      <c r="AK135">
+        <v>-1.027809502865527</v>
+      </c>
     </row>
-    <row r="136" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
-        <v>157</v>
+        <v>167</v>
       </c>
       <c r="B136">
         <v>229</v>
@@ -13456,10 +15502,25 @@
         <f t="shared" si="9"/>
         <v>143</v>
       </c>
+      <c r="AG136">
+        <v>-1.0333578721576711</v>
+      </c>
+      <c r="AH136">
+        <v>-0.84900202626924093</v>
+      </c>
+      <c r="AI136">
+        <v>-0.58239912530611582</v>
+      </c>
+      <c r="AJ136">
+        <v>-0.53096358405814204</v>
+      </c>
+      <c r="AK136">
+        <v>-1.037200370733742</v>
+      </c>
     </row>
-    <row r="137" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
-        <v>102</v>
+        <v>168</v>
       </c>
       <c r="B137">
         <v>257</v>
@@ -13547,10 +15608,25 @@
         <f t="shared" si="9"/>
         <v>143</v>
       </c>
+      <c r="AG137">
+        <v>-0.45226747038093829</v>
+      </c>
+      <c r="AH137">
+        <v>-0.54945182286129657</v>
+      </c>
+      <c r="AI137">
+        <v>-0.51224119532961132</v>
+      </c>
+      <c r="AJ137">
+        <v>-0.81948707769004792</v>
+      </c>
+      <c r="AK137">
+        <v>-1.107898665764337</v>
+      </c>
     </row>
-    <row r="138" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
-        <v>55</v>
+        <v>169</v>
       </c>
       <c r="B138">
         <v>400</v>
@@ -13641,10 +15717,25 @@
       <c r="AE138">
         <v>2.39</v>
       </c>
+      <c r="AG138">
+        <v>0.61061459342558444</v>
+      </c>
+      <c r="AH138">
+        <v>1.603145090685127</v>
+      </c>
+      <c r="AI138">
+        <v>0.33246506644206458</v>
+      </c>
+      <c r="AJ138">
+        <v>0.4493056452912455</v>
+      </c>
+      <c r="AK138">
+        <v>-1.1139204073356761</v>
+      </c>
     </row>
-    <row r="139" spans="1:32" ht="19" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:37" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
-        <v>114</v>
+        <v>170</v>
       </c>
       <c r="B139">
         <v>199</v>
@@ -13735,10 +15826,25 @@
       <c r="AD139" s="3">
         <v>46</v>
       </c>
+      <c r="AG139">
+        <v>1.57758590950059</v>
+      </c>
+      <c r="AH139">
+        <v>0.9884904164386108</v>
+      </c>
+      <c r="AI139">
+        <v>1.527657937307505</v>
+      </c>
+      <c r="AJ139">
+        <v>1.130902260488341</v>
+      </c>
+      <c r="AK139">
+        <v>-1.2132791432627721</v>
+      </c>
     </row>
-    <row r="140" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
-        <v>62</v>
+        <v>171</v>
       </c>
       <c r="B140">
         <v>309</v>
@@ -13826,10 +15932,25 @@
         <f t="shared" si="9"/>
         <v>80</v>
       </c>
+      <c r="AG140">
+        <v>-0.41279704891332181</v>
+      </c>
+      <c r="AH140">
+        <v>-6.3183289317470165E-2</v>
+      </c>
+      <c r="AI140">
+        <v>0.70753966565821125</v>
+      </c>
+      <c r="AJ140">
+        <v>0.26878986646000608</v>
+      </c>
+      <c r="AK140">
+        <v>-1.2132791432627721</v>
+      </c>
     </row>
-    <row r="141" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
-        <v>139</v>
+        <v>172</v>
       </c>
       <c r="B141">
         <v>251</v>
@@ -13917,10 +16038,25 @@
         <f t="shared" si="9"/>
         <v>163</v>
       </c>
+      <c r="AG141">
+        <v>-0.1088213338299011</v>
+      </c>
+      <c r="AH141">
+        <v>6.3225870092886327E-2</v>
+      </c>
+      <c r="AI141">
+        <v>8.6164677999399003E-2</v>
+      </c>
+      <c r="AJ141">
+        <v>-1.001946208207269</v>
+      </c>
+      <c r="AK141">
+        <v>-1.2132791432627721</v>
+      </c>
     </row>
-    <row r="142" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
-        <v>32</v>
+        <v>119</v>
       </c>
       <c r="B142">
         <v>363</v>
@@ -14011,9 +16147,24 @@
       <c r="AF142">
         <v>38.700000000000003</v>
       </c>
+      <c r="AG142">
+        <v>0.34586942548783822</v>
+      </c>
+      <c r="AH142">
+        <v>-0.86721223681275739</v>
+      </c>
+      <c r="AI142">
+        <v>-1.0731000334693499</v>
+      </c>
+      <c r="AJ142">
+        <v>-1.0131337803125611</v>
+      </c>
+      <c r="AK142">
+        <v>-1.2132791432627721</v>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AC142" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <autoFilter ref="A1:AC142" xr:uid="{00000000-0009-0000-0000-000000000000}">
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:AC142">
       <sortCondition descending="1" ref="T1:T142"/>
     </sortState>

</xml_diff>